<commit_message>
--> Golden master of v2.6.0: Awaiting final tests on hardware before release. --> Fixed issue with reading status register 2 and the Suspend operation where the library was not checking the suspend status correctly.
</commit_message>
<xml_diff>
--- a/extras/Library speed comparisons.xlsx
+++ b/extras/Library speed comparisons.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal Bhattaram\Documents\GitHub\SPIFlash\extras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal Bhattaram\Dropbox\Genesis share\Arduino\sketches\libraries\SPIFlash\extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="465" windowWidth="28800" windowHeight="17595" tabRatio="500"/>
+    <workbookView xWindow="8940" yWindow="465" windowWidth="28800" windowHeight="17595" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arduino Due" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="148">
   <si>
     <t>Function</t>
   </si>
@@ -429,6 +429,54 @@
   </si>
   <si>
     <t>204 µs</t>
+  </si>
+  <si>
+    <t>v2.6.0</t>
+  </si>
+  <si>
+    <t>200 µs</t>
+  </si>
+  <si>
+    <t>936 µs</t>
+  </si>
+  <si>
+    <t>416 µs</t>
+  </si>
+  <si>
+    <t>432 µs</t>
+  </si>
+  <si>
+    <t>216 µs</t>
+  </si>
+  <si>
+    <t>512 µs</t>
+  </si>
+  <si>
+    <t>7040 µs</t>
+  </si>
+  <si>
+    <t>1616 µs</t>
+  </si>
+  <si>
+    <t>4536 µs</t>
+  </si>
+  <si>
+    <t>1544 µs</t>
+  </si>
+  <si>
+    <t>48 µs</t>
+  </si>
+  <si>
+    <t>15.1730 ms</t>
+  </si>
+  <si>
+    <t>36.9280 ms</t>
+  </si>
+  <si>
+    <t>44.4770 ms</t>
+  </si>
+  <si>
+    <t>1.2855 s</t>
   </si>
 </sst>
 </file>
@@ -1354,6 +1402,160 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1408,160 +1610,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1854,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1865,94 +1913,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="37.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="197" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146" t="s">
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="198" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
-      <c r="O1" s="146"/>
-      <c r="P1" s="146"/>
-      <c r="Q1" s="146"/>
-      <c r="R1" s="147"/>
+      <c r="K1" s="198"/>
+      <c r="L1" s="198"/>
+      <c r="M1" s="198"/>
+      <c r="N1" s="198"/>
+      <c r="O1" s="198"/>
+      <c r="P1" s="198"/>
+      <c r="Q1" s="198"/>
+      <c r="R1" s="199"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="200" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="154" t="s">
+      <c r="B2" s="201"/>
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
+      <c r="E2" s="206" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="154"/>
-      <c r="P2" s="154"/>
-      <c r="Q2" s="154"/>
-      <c r="R2" s="155"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="206"/>
+      <c r="I2" s="206"/>
+      <c r="J2" s="206"/>
+      <c r="K2" s="206"/>
+      <c r="L2" s="206"/>
+      <c r="M2" s="206"/>
+      <c r="N2" s="206"/>
+      <c r="O2" s="206"/>
+      <c r="P2" s="206"/>
+      <c r="Q2" s="206"/>
+      <c r="R2" s="207"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="150"/>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
-      <c r="M3" s="156"/>
-      <c r="N3" s="156"/>
-      <c r="O3" s="156"/>
-      <c r="P3" s="156"/>
-      <c r="Q3" s="156"/>
-      <c r="R3" s="157"/>
+      <c r="A3" s="202"/>
+      <c r="B3" s="203"/>
+      <c r="C3" s="203"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="208"/>
+      <c r="F3" s="208"/>
+      <c r="G3" s="208"/>
+      <c r="H3" s="208"/>
+      <c r="I3" s="208"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="208"/>
+      <c r="L3" s="208"/>
+      <c r="M3" s="208"/>
+      <c r="N3" s="208"/>
+      <c r="O3" s="208"/>
+      <c r="P3" s="208"/>
+      <c r="Q3" s="208"/>
+      <c r="R3" s="209"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="152"/>
-      <c r="B4" s="153"/>
-      <c r="C4" s="153"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="158" t="s">
+      <c r="A4" s="204"/>
+      <c r="B4" s="205"/>
+      <c r="C4" s="205"/>
+      <c r="D4" s="205"/>
+      <c r="E4" s="210" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="159"/>
-      <c r="G4" s="159"/>
-      <c r="H4" s="159"/>
-      <c r="I4" s="159"/>
-      <c r="J4" s="159"/>
-      <c r="K4" s="159"/>
-      <c r="L4" s="159"/>
-      <c r="M4" s="159"/>
-      <c r="N4" s="159"/>
-      <c r="O4" s="159"/>
-      <c r="P4" s="159"/>
-      <c r="Q4" s="159"/>
-      <c r="R4" s="160"/>
+      <c r="F4" s="211"/>
+      <c r="G4" s="211"/>
+      <c r="H4" s="211"/>
+      <c r="I4" s="211"/>
+      <c r="J4" s="211"/>
+      <c r="K4" s="211"/>
+      <c r="L4" s="211"/>
+      <c r="M4" s="211"/>
+      <c r="N4" s="211"/>
+      <c r="O4" s="211"/>
+      <c r="P4" s="211"/>
+      <c r="Q4" s="211"/>
+      <c r="R4" s="212"/>
     </row>
     <row r="5" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
@@ -1974,7 +2022,9 @@
       <c r="I5" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="141"/>
+      <c r="J5" s="141" t="s">
+        <v>132</v>
+      </c>
       <c r="K5" s="141"/>
       <c r="L5" s="141"/>
       <c r="M5" s="141"/>
@@ -1985,13 +2035,13 @@
       <c r="R5" s="142"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="143" t="s">
+      <c r="A6" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="144">
+      <c r="C6" s="196">
         <v>8</v>
       </c>
       <c r="D6" s="111" t="s">
@@ -2015,9 +2065,9 @@
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="143"/>
-      <c r="B7" s="144"/>
-      <c r="C7" s="144"/>
+      <c r="A7" s="195"/>
+      <c r="B7" s="196"/>
+      <c r="C7" s="196"/>
       <c r="D7" s="112" t="s">
         <v>19</v>
       </c>
@@ -2039,9 +2089,9 @@
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="143"/>
-      <c r="B8" s="144"/>
-      <c r="C8" s="144"/>
+      <c r="A8" s="195"/>
+      <c r="B8" s="196"/>
+      <c r="C8" s="196"/>
       <c r="D8" s="112" t="s">
         <v>21</v>
       </c>
@@ -2063,9 +2113,9 @@
       <c r="R8" s="5"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="143"/>
-      <c r="B9" s="144"/>
-      <c r="C9" s="144"/>
+      <c r="A9" s="195"/>
+      <c r="B9" s="196"/>
+      <c r="C9" s="196"/>
       <c r="D9" s="113" t="s">
         <v>22</v>
       </c>
@@ -2087,13 +2137,13 @@
       <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="161" t="s">
+      <c r="A10" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="162" t="s">
+      <c r="B10" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="162">
+      <c r="C10" s="192">
         <v>8</v>
       </c>
       <c r="D10" s="114" t="s">
@@ -2117,9 +2167,9 @@
       <c r="R10" s="9"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="161"/>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
+      <c r="A11" s="191"/>
+      <c r="B11" s="192"/>
+      <c r="C11" s="192"/>
       <c r="D11" s="115" t="s">
         <v>19</v>
       </c>
@@ -2141,9 +2191,9 @@
       <c r="R11" s="11"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="161"/>
-      <c r="B12" s="162"/>
-      <c r="C12" s="162"/>
+      <c r="A12" s="191"/>
+      <c r="B12" s="192"/>
+      <c r="C12" s="192"/>
       <c r="D12" s="115" t="s">
         <v>21</v>
       </c>
@@ -2165,9 +2215,9 @@
       <c r="R12" s="11"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="161"/>
-      <c r="B13" s="162"/>
-      <c r="C13" s="162"/>
+      <c r="A13" s="191"/>
+      <c r="B13" s="192"/>
+      <c r="C13" s="192"/>
       <c r="D13" s="116" t="s">
         <v>22</v>
       </c>
@@ -2189,13 +2239,13 @@
       <c r="R13" s="13"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="163" t="s">
+      <c r="A14" s="193" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="164">
+      <c r="C14" s="194">
         <v>16</v>
       </c>
       <c r="D14" s="117" t="s">
@@ -2219,9 +2269,9 @@
       <c r="R14" s="15"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="163"/>
-      <c r="B15" s="164"/>
-      <c r="C15" s="164"/>
+      <c r="A15" s="193"/>
+      <c r="B15" s="194"/>
+      <c r="C15" s="194"/>
       <c r="D15" s="118" t="s">
         <v>19</v>
       </c>
@@ -2243,9 +2293,9 @@
       <c r="R15" s="17"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="163"/>
-      <c r="B16" s="164"/>
-      <c r="C16" s="164"/>
+      <c r="A16" s="193"/>
+      <c r="B16" s="194"/>
+      <c r="C16" s="194"/>
       <c r="D16" s="118" t="s">
         <v>21</v>
       </c>
@@ -2267,9 +2317,9 @@
       <c r="R16" s="17"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="163"/>
-      <c r="B17" s="164"/>
-      <c r="C17" s="164"/>
+      <c r="A17" s="193"/>
+      <c r="B17" s="194"/>
+      <c r="C17" s="194"/>
       <c r="D17" s="119" t="s">
         <v>22</v>
       </c>
@@ -2291,13 +2341,13 @@
       <c r="R17" s="19"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="165" t="s">
+      <c r="A18" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="166" t="s">
+      <c r="B18" s="188" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="166">
+      <c r="C18" s="188">
         <v>16</v>
       </c>
       <c r="D18" s="120" t="s">
@@ -2321,9 +2371,9 @@
       <c r="R18" s="21"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="165"/>
-      <c r="B19" s="166"/>
-      <c r="C19" s="166"/>
+      <c r="A19" s="187"/>
+      <c r="B19" s="188"/>
+      <c r="C19" s="188"/>
       <c r="D19" s="121" t="s">
         <v>19</v>
       </c>
@@ -2345,9 +2395,9 @@
       <c r="R19" s="23"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="165"/>
-      <c r="B20" s="166"/>
-      <c r="C20" s="166"/>
+      <c r="A20" s="187"/>
+      <c r="B20" s="188"/>
+      <c r="C20" s="188"/>
       <c r="D20" s="121" t="s">
         <v>21</v>
       </c>
@@ -2369,9 +2419,9 @@
       <c r="R20" s="23"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="165"/>
-      <c r="B21" s="166"/>
-      <c r="C21" s="166"/>
+      <c r="A21" s="187"/>
+      <c r="B21" s="188"/>
+      <c r="C21" s="188"/>
       <c r="D21" s="122" t="s">
         <v>22</v>
       </c>
@@ -2393,13 +2443,13 @@
       <c r="R21" s="25"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="167" t="s">
+      <c r="A22" s="189" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="168" t="s">
+      <c r="B22" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="168">
+      <c r="C22" s="190">
         <v>32</v>
       </c>
       <c r="D22" s="123" t="s">
@@ -2423,9 +2473,9 @@
       <c r="R22" s="27"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="167"/>
-      <c r="B23" s="168"/>
-      <c r="C23" s="168"/>
+      <c r="A23" s="189"/>
+      <c r="B23" s="190"/>
+      <c r="C23" s="190"/>
       <c r="D23" s="124" t="s">
         <v>19</v>
       </c>
@@ -2447,9 +2497,9 @@
       <c r="R23" s="29"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="167"/>
-      <c r="B24" s="168"/>
-      <c r="C24" s="168"/>
+      <c r="A24" s="189"/>
+      <c r="B24" s="190"/>
+      <c r="C24" s="190"/>
       <c r="D24" s="124" t="s">
         <v>21</v>
       </c>
@@ -2471,9 +2521,9 @@
       <c r="R24" s="29"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="167"/>
-      <c r="B25" s="168"/>
-      <c r="C25" s="168"/>
+      <c r="A25" s="189"/>
+      <c r="B25" s="190"/>
+      <c r="C25" s="190"/>
       <c r="D25" s="125" t="s">
         <v>22</v>
       </c>
@@ -2495,13 +2545,13 @@
       <c r="R25" s="31"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="169" t="s">
+      <c r="A26" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="170" t="s">
+      <c r="B26" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="170">
+      <c r="C26" s="184">
         <v>32</v>
       </c>
       <c r="D26" s="126" t="s">
@@ -2525,9 +2575,9 @@
       <c r="R26" s="33"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="169"/>
-      <c r="B27" s="170"/>
-      <c r="C27" s="170"/>
+      <c r="A27" s="183"/>
+      <c r="B27" s="184"/>
+      <c r="C27" s="184"/>
       <c r="D27" s="127" t="s">
         <v>19</v>
       </c>
@@ -2549,9 +2599,9 @@
       <c r="R27" s="35"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="169"/>
-      <c r="B28" s="170"/>
-      <c r="C28" s="170"/>
+      <c r="A28" s="183"/>
+      <c r="B28" s="184"/>
+      <c r="C28" s="184"/>
       <c r="D28" s="127" t="s">
         <v>21</v>
       </c>
@@ -2573,9 +2623,9 @@
       <c r="R28" s="35"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="169"/>
-      <c r="B29" s="170"/>
-      <c r="C29" s="170"/>
+      <c r="A29" s="183"/>
+      <c r="B29" s="184"/>
+      <c r="C29" s="184"/>
       <c r="D29" s="128" t="s">
         <v>22</v>
       </c>
@@ -2597,13 +2647,13 @@
       <c r="R29" s="37"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="171" t="s">
+      <c r="A30" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="172" t="s">
+      <c r="B30" s="186" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="172">
+      <c r="C30" s="186">
         <v>32</v>
       </c>
       <c r="D30" s="129" t="s">
@@ -2627,9 +2677,9 @@
       <c r="R30" s="39"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="171"/>
-      <c r="B31" s="172"/>
-      <c r="C31" s="172"/>
+      <c r="A31" s="185"/>
+      <c r="B31" s="186"/>
+      <c r="C31" s="186"/>
       <c r="D31" s="130" t="s">
         <v>19</v>
       </c>
@@ -2651,9 +2701,9 @@
       <c r="R31" s="41"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="171"/>
-      <c r="B32" s="172"/>
-      <c r="C32" s="172"/>
+      <c r="A32" s="185"/>
+      <c r="B32" s="186"/>
+      <c r="C32" s="186"/>
       <c r="D32" s="130" t="s">
         <v>21</v>
       </c>
@@ -2675,9 +2725,9 @@
       <c r="R32" s="41"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="171"/>
-      <c r="B33" s="172"/>
-      <c r="C33" s="172"/>
+      <c r="A33" s="185"/>
+      <c r="B33" s="186"/>
+      <c r="C33" s="186"/>
       <c r="D33" s="131" t="s">
         <v>22</v>
       </c>
@@ -2699,13 +2749,13 @@
       <c r="R33" s="55"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="173" t="s">
+      <c r="A34" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="174" t="s">
+      <c r="B34" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="175" t="s">
+      <c r="C34" s="179" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="132" t="s">
@@ -2729,9 +2779,9 @@
       <c r="R34" s="43"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="173"/>
-      <c r="B35" s="174"/>
-      <c r="C35" s="175"/>
+      <c r="A35" s="177"/>
+      <c r="B35" s="178"/>
+      <c r="C35" s="179"/>
       <c r="D35" s="133" t="s">
         <v>19</v>
       </c>
@@ -2753,9 +2803,9 @@
       <c r="R35" s="45"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="173"/>
-      <c r="B36" s="174"/>
-      <c r="C36" s="175"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="178"/>
+      <c r="C36" s="179"/>
       <c r="D36" s="133" t="s">
         <v>21</v>
       </c>
@@ -2777,9 +2827,9 @@
       <c r="R36" s="45"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="173"/>
-      <c r="B37" s="174"/>
-      <c r="C37" s="174"/>
+      <c r="A37" s="177"/>
+      <c r="B37" s="178"/>
+      <c r="C37" s="178"/>
       <c r="D37" s="134" t="s">
         <v>22</v>
       </c>
@@ -2801,13 +2851,13 @@
       <c r="R37" s="57"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="176" t="s">
+      <c r="A38" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="177" t="s">
+      <c r="B38" s="181" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="178" t="s">
+      <c r="C38" s="182" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="135" t="s">
@@ -2831,9 +2881,9 @@
       <c r="R38" s="47"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="176"/>
-      <c r="B39" s="177"/>
-      <c r="C39" s="178"/>
+      <c r="A39" s="180"/>
+      <c r="B39" s="181"/>
+      <c r="C39" s="182"/>
       <c r="D39" s="136" t="s">
         <v>19</v>
       </c>
@@ -2855,9 +2905,9 @@
       <c r="R39" s="49"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="176"/>
-      <c r="B40" s="177"/>
-      <c r="C40" s="178"/>
+      <c r="A40" s="180"/>
+      <c r="B40" s="181"/>
+      <c r="C40" s="182"/>
       <c r="D40" s="136" t="s">
         <v>21</v>
       </c>
@@ -2879,9 +2929,9 @@
       <c r="R40" s="49"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="176"/>
-      <c r="B41" s="177"/>
-      <c r="C41" s="177"/>
+      <c r="A41" s="180"/>
+      <c r="B41" s="181"/>
+      <c r="C41" s="181"/>
       <c r="D41" s="137" t="s">
         <v>22</v>
       </c>
@@ -2903,13 +2953,13 @@
       <c r="R41" s="59"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="179" t="s">
+      <c r="A42" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="181" t="s">
+      <c r="B42" s="170" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="182" t="s">
+      <c r="C42" s="171" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="138" t="s">
@@ -2933,9 +2983,9 @@
       <c r="R42" s="51"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="179"/>
-      <c r="B43" s="181"/>
-      <c r="C43" s="182"/>
+      <c r="A43" s="168"/>
+      <c r="B43" s="170"/>
+      <c r="C43" s="171"/>
       <c r="D43" s="139" t="s">
         <v>19</v>
       </c>
@@ -2957,9 +3007,9 @@
       <c r="R43" s="53"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="179"/>
-      <c r="B44" s="181"/>
-      <c r="C44" s="182"/>
+      <c r="A44" s="168"/>
+      <c r="B44" s="170"/>
+      <c r="C44" s="171"/>
       <c r="D44" s="139" t="s">
         <v>21</v>
       </c>
@@ -2981,9 +3031,9 @@
       <c r="R44" s="53"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="180"/>
-      <c r="B45" s="181"/>
-      <c r="C45" s="181"/>
+      <c r="A45" s="169"/>
+      <c r="B45" s="170"/>
+      <c r="C45" s="170"/>
       <c r="D45" s="139" t="s">
         <v>22</v>
       </c>
@@ -3005,56 +3055,56 @@
       <c r="R45" s="53"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="183" t="s">
+      <c r="A46" s="172" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="184"/>
-      <c r="C46" s="184"/>
-      <c r="D46" s="185"/>
-      <c r="E46" s="186"/>
-      <c r="F46" s="188"/>
-      <c r="G46" s="188"/>
-      <c r="H46" s="188"/>
-      <c r="I46" s="192" t="s">
+      <c r="B46" s="173"/>
+      <c r="C46" s="173"/>
+      <c r="D46" s="174"/>
+      <c r="E46" s="175"/>
+      <c r="F46" s="147"/>
+      <c r="G46" s="147"/>
+      <c r="H46" s="147"/>
+      <c r="I46" s="166" t="s">
         <v>1</v>
       </c>
-      <c r="J46" s="188"/>
-      <c r="K46" s="188"/>
-      <c r="L46" s="188"/>
-      <c r="M46" s="188"/>
-      <c r="N46" s="188"/>
-      <c r="O46" s="188"/>
-      <c r="P46" s="188"/>
-      <c r="Q46" s="188"/>
-      <c r="R46" s="190"/>
+      <c r="J46" s="147"/>
+      <c r="K46" s="147"/>
+      <c r="L46" s="147"/>
+      <c r="M46" s="147"/>
+      <c r="N46" s="147"/>
+      <c r="O46" s="147"/>
+      <c r="P46" s="147"/>
+      <c r="Q46" s="147"/>
+      <c r="R46" s="164"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="183"/>
-      <c r="B47" s="184"/>
-      <c r="C47" s="184"/>
-      <c r="D47" s="185"/>
-      <c r="E47" s="187"/>
-      <c r="F47" s="189"/>
-      <c r="G47" s="189"/>
-      <c r="H47" s="189"/>
-      <c r="I47" s="193"/>
-      <c r="J47" s="189"/>
-      <c r="K47" s="189"/>
-      <c r="L47" s="189"/>
-      <c r="M47" s="189"/>
-      <c r="N47" s="189"/>
-      <c r="O47" s="189"/>
-      <c r="P47" s="189"/>
-      <c r="Q47" s="189"/>
-      <c r="R47" s="191"/>
+      <c r="A47" s="172"/>
+      <c r="B47" s="173"/>
+      <c r="C47" s="173"/>
+      <c r="D47" s="174"/>
+      <c r="E47" s="176"/>
+      <c r="F47" s="148"/>
+      <c r="G47" s="148"/>
+      <c r="H47" s="148"/>
+      <c r="I47" s="167"/>
+      <c r="J47" s="148"/>
+      <c r="K47" s="148"/>
+      <c r="L47" s="148"/>
+      <c r="M47" s="148"/>
+      <c r="N47" s="148"/>
+      <c r="O47" s="148"/>
+      <c r="P47" s="148"/>
+      <c r="Q47" s="148"/>
+      <c r="R47" s="165"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="197" t="s">
+      <c r="A48" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="198"/>
-      <c r="C48" s="198"/>
-      <c r="D48" s="199"/>
+      <c r="B48" s="150"/>
+      <c r="C48" s="150"/>
+      <c r="D48" s="151"/>
       <c r="E48" s="104"/>
       <c r="F48" s="65"/>
       <c r="G48" s="65"/>
@@ -3073,12 +3123,12 @@
       <c r="R48" s="66"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="200" t="s">
+      <c r="A49" s="152" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="201"/>
-      <c r="C49" s="201"/>
-      <c r="D49" s="202"/>
+      <c r="B49" s="153"/>
+      <c r="C49" s="153"/>
+      <c r="D49" s="154"/>
       <c r="E49" s="105"/>
       <c r="F49" s="63"/>
       <c r="G49" s="63"/>
@@ -3097,12 +3147,12 @@
       <c r="R49" s="64"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="203" t="s">
+      <c r="A50" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="204"/>
-      <c r="C50" s="204"/>
-      <c r="D50" s="205"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="156"/>
+      <c r="D50" s="157"/>
       <c r="E50" s="106"/>
       <c r="F50" s="67"/>
       <c r="G50" s="67"/>
@@ -3121,12 +3171,12 @@
       <c r="R50" s="68"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="206" t="s">
+      <c r="A51" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="207"/>
-      <c r="C51" s="207"/>
-      <c r="D51" s="208"/>
+      <c r="B51" s="159"/>
+      <c r="C51" s="159"/>
+      <c r="D51" s="160"/>
       <c r="E51" s="107"/>
       <c r="F51" s="69"/>
       <c r="G51" s="69"/>
@@ -3145,12 +3195,12 @@
       <c r="R51" s="70"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="209" t="s">
+      <c r="A52" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="210"/>
-      <c r="C52" s="210"/>
-      <c r="D52" s="211"/>
+      <c r="B52" s="162"/>
+      <c r="C52" s="162"/>
+      <c r="D52" s="163"/>
       <c r="E52" s="108"/>
       <c r="F52" s="71"/>
       <c r="G52" s="71"/>
@@ -3169,12 +3219,12 @@
       <c r="R52" s="72"/>
     </row>
     <row r="53" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="194" t="s">
+      <c r="A53" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="195"/>
-      <c r="C53" s="195"/>
-      <c r="D53" s="196"/>
+      <c r="B53" s="145"/>
+      <c r="C53" s="145"/>
+      <c r="D53" s="146"/>
       <c r="E53" s="109"/>
       <c r="F53" s="73"/>
       <c r="G53" s="73"/>
@@ -3195,6 +3245,51 @@
     <row r="54" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="A2:D4"/>
+    <mergeCell ref="E2:R3"/>
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="A46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="Q46:Q47"/>
+    <mergeCell ref="R46:R47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="H46:H47"/>
+    <mergeCell ref="I46:I47"/>
+    <mergeCell ref="J46:J47"/>
+    <mergeCell ref="K46:K47"/>
+    <mergeCell ref="L46:L47"/>
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="M46:M47"/>
     <mergeCell ref="N46:N47"/>
@@ -3206,51 +3301,6 @@
     <mergeCell ref="A50:D50"/>
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A52:D52"/>
-    <mergeCell ref="Q46:Q47"/>
-    <mergeCell ref="R46:R47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="H46:H47"/>
-    <mergeCell ref="I46:I47"/>
-    <mergeCell ref="J46:J47"/>
-    <mergeCell ref="K46:K47"/>
-    <mergeCell ref="L46:L47"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="A46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:R1"/>
-    <mergeCell ref="A2:D4"/>
-    <mergeCell ref="E2:R3"/>
-    <mergeCell ref="E4:R4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3260,8 +3310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="F34" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3271,94 +3321,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="37.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="197" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146" t="s">
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="198" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
-      <c r="O1" s="146"/>
-      <c r="P1" s="146"/>
-      <c r="Q1" s="146"/>
-      <c r="R1" s="147"/>
+      <c r="K1" s="198"/>
+      <c r="L1" s="198"/>
+      <c r="M1" s="198"/>
+      <c r="N1" s="198"/>
+      <c r="O1" s="198"/>
+      <c r="P1" s="198"/>
+      <c r="Q1" s="198"/>
+      <c r="R1" s="199"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="200" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="154" t="s">
+      <c r="B2" s="201"/>
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
+      <c r="E2" s="206" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="154"/>
-      <c r="P2" s="154"/>
-      <c r="Q2" s="154"/>
-      <c r="R2" s="155"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="206"/>
+      <c r="I2" s="206"/>
+      <c r="J2" s="206"/>
+      <c r="K2" s="206"/>
+      <c r="L2" s="206"/>
+      <c r="M2" s="206"/>
+      <c r="N2" s="206"/>
+      <c r="O2" s="206"/>
+      <c r="P2" s="206"/>
+      <c r="Q2" s="206"/>
+      <c r="R2" s="207"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="150"/>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
-      <c r="M3" s="156"/>
-      <c r="N3" s="156"/>
-      <c r="O3" s="156"/>
-      <c r="P3" s="156"/>
-      <c r="Q3" s="156"/>
-      <c r="R3" s="157"/>
+      <c r="A3" s="202"/>
+      <c r="B3" s="203"/>
+      <c r="C3" s="203"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="208"/>
+      <c r="F3" s="208"/>
+      <c r="G3" s="208"/>
+      <c r="H3" s="208"/>
+      <c r="I3" s="208"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="208"/>
+      <c r="L3" s="208"/>
+      <c r="M3" s="208"/>
+      <c r="N3" s="208"/>
+      <c r="O3" s="208"/>
+      <c r="P3" s="208"/>
+      <c r="Q3" s="208"/>
+      <c r="R3" s="209"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="152"/>
-      <c r="B4" s="153"/>
-      <c r="C4" s="153"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="158" t="s">
+      <c r="A4" s="204"/>
+      <c r="B4" s="205"/>
+      <c r="C4" s="205"/>
+      <c r="D4" s="205"/>
+      <c r="E4" s="210" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="159"/>
-      <c r="G4" s="159"/>
-      <c r="H4" s="159"/>
-      <c r="I4" s="159"/>
-      <c r="J4" s="159"/>
-      <c r="K4" s="159"/>
-      <c r="L4" s="159"/>
-      <c r="M4" s="159"/>
-      <c r="N4" s="159"/>
-      <c r="O4" s="159"/>
-      <c r="P4" s="159"/>
-      <c r="Q4" s="159"/>
-      <c r="R4" s="160"/>
+      <c r="F4" s="211"/>
+      <c r="G4" s="211"/>
+      <c r="H4" s="211"/>
+      <c r="I4" s="211"/>
+      <c r="J4" s="211"/>
+      <c r="K4" s="211"/>
+      <c r="L4" s="211"/>
+      <c r="M4" s="211"/>
+      <c r="N4" s="211"/>
+      <c r="O4" s="211"/>
+      <c r="P4" s="211"/>
+      <c r="Q4" s="211"/>
+      <c r="R4" s="212"/>
     </row>
     <row r="5" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
@@ -3380,7 +3430,9 @@
       <c r="I5" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="141"/>
+      <c r="J5" s="141" t="s">
+        <v>132</v>
+      </c>
       <c r="K5" s="141"/>
       <c r="L5" s="141"/>
       <c r="M5" s="141"/>
@@ -3391,13 +3443,13 @@
       <c r="R5" s="142"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="143" t="s">
+      <c r="A6" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="144">
+      <c r="C6" s="196">
         <v>8</v>
       </c>
       <c r="D6" s="111" t="s">
@@ -3407,10 +3459,12 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="212" t="s">
+      <c r="I6" s="143" t="s">
         <v>72</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -3421,9 +3475,9 @@
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="143"/>
-      <c r="B7" s="144"/>
-      <c r="C7" s="144"/>
+      <c r="A7" s="195"/>
+      <c r="B7" s="196"/>
+      <c r="C7" s="196"/>
       <c r="D7" s="112" t="s">
         <v>19</v>
       </c>
@@ -3434,7 +3488,9 @@
       <c r="I7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="4"/>
+      <c r="J7" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -3445,9 +3501,9 @@
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="143"/>
-      <c r="B8" s="144"/>
-      <c r="C8" s="144"/>
+      <c r="A8" s="195"/>
+      <c r="B8" s="196"/>
+      <c r="C8" s="196"/>
       <c r="D8" s="112" t="s">
         <v>21</v>
       </c>
@@ -3458,7 +3514,9 @@
       <c r="I8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -3469,9 +3527,9 @@
       <c r="R8" s="5"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="143"/>
-      <c r="B9" s="144"/>
-      <c r="C9" s="144"/>
+      <c r="A9" s="195"/>
+      <c r="B9" s="196"/>
+      <c r="C9" s="196"/>
       <c r="D9" s="113" t="s">
         <v>22</v>
       </c>
@@ -3482,7 +3540,9 @@
       <c r="I9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
@@ -3493,13 +3553,13 @@
       <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="161" t="s">
+      <c r="A10" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="162" t="s">
+      <c r="B10" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="162">
+      <c r="C10" s="192">
         <v>8</v>
       </c>
       <c r="D10" s="114" t="s">
@@ -3512,7 +3572,9 @@
       <c r="I10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="8"/>
+      <c r="J10" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
@@ -3523,9 +3585,9 @@
       <c r="R10" s="9"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="161"/>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
+      <c r="A11" s="191"/>
+      <c r="B11" s="192"/>
+      <c r="C11" s="192"/>
       <c r="D11" s="115" t="s">
         <v>19</v>
       </c>
@@ -3536,7 +3598,9 @@
       <c r="I11" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="J11" s="10"/>
+      <c r="J11" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
@@ -3547,9 +3611,9 @@
       <c r="R11" s="11"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="161"/>
-      <c r="B12" s="162"/>
-      <c r="C12" s="162"/>
+      <c r="A12" s="191"/>
+      <c r="B12" s="192"/>
+      <c r="C12" s="192"/>
       <c r="D12" s="115" t="s">
         <v>21</v>
       </c>
@@ -3560,7 +3624,9 @@
       <c r="I12" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J12" s="10"/>
+      <c r="J12" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
@@ -3571,9 +3637,9 @@
       <c r="R12" s="11"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="161"/>
-      <c r="B13" s="162"/>
-      <c r="C13" s="162"/>
+      <c r="A13" s="191"/>
+      <c r="B13" s="192"/>
+      <c r="C13" s="192"/>
       <c r="D13" s="116" t="s">
         <v>22</v>
       </c>
@@ -3584,7 +3650,9 @@
       <c r="I13" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="12"/>
+      <c r="J13" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
@@ -3595,13 +3663,13 @@
       <c r="R13" s="13"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="163" t="s">
+      <c r="A14" s="193" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="164">
+      <c r="C14" s="194">
         <v>16</v>
       </c>
       <c r="D14" s="117" t="s">
@@ -3614,7 +3682,9 @@
       <c r="I14" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="J14" s="14"/>
+      <c r="J14" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
@@ -3625,9 +3695,9 @@
       <c r="R14" s="15"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="163"/>
-      <c r="B15" s="164"/>
-      <c r="C15" s="164"/>
+      <c r="A15" s="193"/>
+      <c r="B15" s="194"/>
+      <c r="C15" s="194"/>
       <c r="D15" s="118" t="s">
         <v>19</v>
       </c>
@@ -3638,7 +3708,9 @@
       <c r="I15" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="16"/>
+      <c r="J15" s="16" t="s">
+        <v>79</v>
+      </c>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
@@ -3649,9 +3721,9 @@
       <c r="R15" s="17"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="163"/>
-      <c r="B16" s="164"/>
-      <c r="C16" s="164"/>
+      <c r="A16" s="193"/>
+      <c r="B16" s="194"/>
+      <c r="C16" s="194"/>
       <c r="D16" s="118" t="s">
         <v>21</v>
       </c>
@@ -3662,7 +3734,9 @@
       <c r="I16" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="16"/>
+      <c r="J16" s="16" t="s">
+        <v>78</v>
+      </c>
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
@@ -3673,9 +3747,9 @@
       <c r="R16" s="17"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="163"/>
-      <c r="B17" s="164"/>
-      <c r="C17" s="164"/>
+      <c r="A17" s="193"/>
+      <c r="B17" s="194"/>
+      <c r="C17" s="194"/>
       <c r="D17" s="119" t="s">
         <v>22</v>
       </c>
@@ -3686,7 +3760,9 @@
       <c r="I17" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J17" s="18"/>
+      <c r="J17" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
@@ -3697,13 +3773,13 @@
       <c r="R17" s="19"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="165" t="s">
+      <c r="A18" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="166" t="s">
+      <c r="B18" s="188" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="166">
+      <c r="C18" s="188">
         <v>16</v>
       </c>
       <c r="D18" s="120" t="s">
@@ -3716,7 +3792,9 @@
       <c r="I18" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="J18" s="20"/>
+      <c r="J18" s="20" t="s">
+        <v>76</v>
+      </c>
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
@@ -3727,9 +3805,9 @@
       <c r="R18" s="21"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="165"/>
-      <c r="B19" s="166"/>
-      <c r="C19" s="166"/>
+      <c r="A19" s="187"/>
+      <c r="B19" s="188"/>
+      <c r="C19" s="188"/>
       <c r="D19" s="121" t="s">
         <v>19</v>
       </c>
@@ -3740,7 +3818,9 @@
       <c r="I19" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="J19" s="22"/>
+      <c r="J19" s="22" t="s">
+        <v>79</v>
+      </c>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
@@ -3751,9 +3831,9 @@
       <c r="R19" s="23"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="165"/>
-      <c r="B20" s="166"/>
-      <c r="C20" s="166"/>
+      <c r="A20" s="187"/>
+      <c r="B20" s="188"/>
+      <c r="C20" s="188"/>
       <c r="D20" s="121" t="s">
         <v>21</v>
       </c>
@@ -3764,7 +3844,9 @@
       <c r="I20" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="J20" s="22"/>
+      <c r="J20" s="22" t="s">
+        <v>78</v>
+      </c>
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
       <c r="M20" s="22"/>
@@ -3775,9 +3857,9 @@
       <c r="R20" s="23"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="165"/>
-      <c r="B21" s="166"/>
-      <c r="C21" s="166"/>
+      <c r="A21" s="187"/>
+      <c r="B21" s="188"/>
+      <c r="C21" s="188"/>
       <c r="D21" s="122" t="s">
         <v>22</v>
       </c>
@@ -3788,7 +3870,9 @@
       <c r="I21" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="J21" s="24"/>
+      <c r="J21" s="24" t="s">
+        <v>36</v>
+      </c>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
@@ -3799,13 +3883,13 @@
       <c r="R21" s="25"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="167" t="s">
+      <c r="A22" s="189" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="168" t="s">
+      <c r="B22" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="168">
+      <c r="C22" s="190">
         <v>32</v>
       </c>
       <c r="D22" s="123" t="s">
@@ -3818,7 +3902,9 @@
       <c r="I22" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="J22" s="26"/>
+      <c r="J22" s="26" t="s">
+        <v>82</v>
+      </c>
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
       <c r="M22" s="26"/>
@@ -3829,9 +3915,9 @@
       <c r="R22" s="27"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="167"/>
-      <c r="B23" s="168"/>
-      <c r="C23" s="168"/>
+      <c r="A23" s="189"/>
+      <c r="B23" s="190"/>
+      <c r="C23" s="190"/>
       <c r="D23" s="124" t="s">
         <v>19</v>
       </c>
@@ -3842,7 +3928,9 @@
       <c r="I23" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="J23" s="28"/>
+      <c r="J23" s="28" t="s">
+        <v>40</v>
+      </c>
       <c r="K23" s="28"/>
       <c r="L23" s="28"/>
       <c r="M23" s="28"/>
@@ -3853,9 +3941,9 @@
       <c r="R23" s="29"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="167"/>
-      <c r="B24" s="168"/>
-      <c r="C24" s="168"/>
+      <c r="A24" s="189"/>
+      <c r="B24" s="190"/>
+      <c r="C24" s="190"/>
       <c r="D24" s="124" t="s">
         <v>21</v>
       </c>
@@ -3866,7 +3954,9 @@
       <c r="I24" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="J24" s="28"/>
+      <c r="J24" s="28" t="s">
+        <v>81</v>
+      </c>
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
@@ -3877,9 +3967,9 @@
       <c r="R24" s="29"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="167"/>
-      <c r="B25" s="168"/>
-      <c r="C25" s="168"/>
+      <c r="A25" s="189"/>
+      <c r="B25" s="190"/>
+      <c r="C25" s="190"/>
       <c r="D25" s="125" t="s">
         <v>22</v>
       </c>
@@ -3890,7 +3980,9 @@
       <c r="I25" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="J25" s="30"/>
+      <c r="J25" s="30" t="s">
+        <v>39</v>
+      </c>
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
       <c r="M25" s="30"/>
@@ -3901,13 +3993,13 @@
       <c r="R25" s="31"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="169" t="s">
+      <c r="A26" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="170" t="s">
+      <c r="B26" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="170">
+      <c r="C26" s="184">
         <v>32</v>
       </c>
       <c r="D26" s="126" t="s">
@@ -3920,7 +4012,9 @@
       <c r="I26" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="J26" s="32"/>
+      <c r="J26" s="32" t="s">
+        <v>82</v>
+      </c>
       <c r="K26" s="32"/>
       <c r="L26" s="32"/>
       <c r="M26" s="32"/>
@@ -3931,9 +4025,9 @@
       <c r="R26" s="33"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="169"/>
-      <c r="B27" s="170"/>
-      <c r="C27" s="170"/>
+      <c r="A27" s="183"/>
+      <c r="B27" s="184"/>
+      <c r="C27" s="184"/>
       <c r="D27" s="127" t="s">
         <v>19</v>
       </c>
@@ -3944,7 +4038,9 @@
       <c r="I27" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="J27" s="34"/>
+      <c r="J27" s="34" t="s">
+        <v>40</v>
+      </c>
       <c r="K27" s="34"/>
       <c r="L27" s="34"/>
       <c r="M27" s="34"/>
@@ -3955,9 +4051,9 @@
       <c r="R27" s="35"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="169"/>
-      <c r="B28" s="170"/>
-      <c r="C28" s="170"/>
+      <c r="A28" s="183"/>
+      <c r="B28" s="184"/>
+      <c r="C28" s="184"/>
       <c r="D28" s="127" t="s">
         <v>21</v>
       </c>
@@ -3968,7 +4064,9 @@
       <c r="I28" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="J28" s="34"/>
+      <c r="J28" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="K28" s="34"/>
       <c r="L28" s="34"/>
       <c r="M28" s="34"/>
@@ -3979,9 +4077,9 @@
       <c r="R28" s="35"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="169"/>
-      <c r="B29" s="170"/>
-      <c r="C29" s="170"/>
+      <c r="A29" s="183"/>
+      <c r="B29" s="184"/>
+      <c r="C29" s="184"/>
       <c r="D29" s="128" t="s">
         <v>22</v>
       </c>
@@ -3992,7 +4090,9 @@
       <c r="I29" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="J29" s="36"/>
+      <c r="J29" s="36" t="s">
+        <v>39</v>
+      </c>
       <c r="K29" s="36"/>
       <c r="L29" s="36"/>
       <c r="M29" s="36"/>
@@ -4003,13 +4103,13 @@
       <c r="R29" s="37"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="171" t="s">
+      <c r="A30" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="172" t="s">
+      <c r="B30" s="186" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="172">
+      <c r="C30" s="186">
         <v>32</v>
       </c>
       <c r="D30" s="129" t="s">
@@ -4022,7 +4122,9 @@
       <c r="I30" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="J30" s="38"/>
+      <c r="J30" s="38" t="s">
+        <v>80</v>
+      </c>
       <c r="K30" s="38"/>
       <c r="L30" s="38"/>
       <c r="M30" s="38"/>
@@ -4033,9 +4135,9 @@
       <c r="R30" s="39"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="171"/>
-      <c r="B31" s="172"/>
-      <c r="C31" s="172"/>
+      <c r="A31" s="185"/>
+      <c r="B31" s="186"/>
+      <c r="C31" s="186"/>
       <c r="D31" s="130" t="s">
         <v>19</v>
       </c>
@@ -4046,7 +4148,9 @@
       <c r="I31" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="J31" s="40"/>
+      <c r="J31" s="40" t="s">
+        <v>40</v>
+      </c>
       <c r="K31" s="40"/>
       <c r="L31" s="40"/>
       <c r="M31" s="40"/>
@@ -4057,9 +4161,9 @@
       <c r="R31" s="41"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="171"/>
-      <c r="B32" s="172"/>
-      <c r="C32" s="172"/>
+      <c r="A32" s="185"/>
+      <c r="B32" s="186"/>
+      <c r="C32" s="186"/>
       <c r="D32" s="130" t="s">
         <v>21</v>
       </c>
@@ -4070,7 +4174,9 @@
       <c r="I32" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="J32" s="40"/>
+      <c r="J32" s="40" t="s">
+        <v>83</v>
+      </c>
       <c r="K32" s="40"/>
       <c r="L32" s="40"/>
       <c r="M32" s="40"/>
@@ -4081,9 +4187,9 @@
       <c r="R32" s="41"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="171"/>
-      <c r="B33" s="172"/>
-      <c r="C33" s="172"/>
+      <c r="A33" s="185"/>
+      <c r="B33" s="186"/>
+      <c r="C33" s="186"/>
       <c r="D33" s="131" t="s">
         <v>22</v>
       </c>
@@ -4094,7 +4200,9 @@
       <c r="I33" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="J33" s="54"/>
+      <c r="J33" s="54" t="s">
+        <v>41</v>
+      </c>
       <c r="K33" s="54"/>
       <c r="L33" s="54"/>
       <c r="M33" s="54"/>
@@ -4105,13 +4213,13 @@
       <c r="R33" s="55"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="173" t="s">
+      <c r="A34" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="174" t="s">
+      <c r="B34" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="175" t="s">
+      <c r="C34" s="179" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="132" t="s">
@@ -4124,7 +4232,9 @@
       <c r="I34" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="J34" s="42"/>
+      <c r="J34" s="42" t="s">
+        <v>134</v>
+      </c>
       <c r="K34" s="42"/>
       <c r="L34" s="42"/>
       <c r="M34" s="42"/>
@@ -4135,9 +4245,9 @@
       <c r="R34" s="43"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="173"/>
-      <c r="B35" s="174"/>
-      <c r="C35" s="175"/>
+      <c r="A35" s="177"/>
+      <c r="B35" s="178"/>
+      <c r="C35" s="179"/>
       <c r="D35" s="133" t="s">
         <v>19</v>
       </c>
@@ -4148,7 +4258,9 @@
       <c r="I35" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="J35" s="44"/>
+      <c r="J35" s="44" t="s">
+        <v>135</v>
+      </c>
       <c r="K35" s="44"/>
       <c r="L35" s="44"/>
       <c r="M35" s="44"/>
@@ -4159,9 +4271,9 @@
       <c r="R35" s="45"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="173"/>
-      <c r="B36" s="174"/>
-      <c r="C36" s="175"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="178"/>
+      <c r="C36" s="179"/>
       <c r="D36" s="133" t="s">
         <v>21</v>
       </c>
@@ -4172,7 +4284,9 @@
       <c r="I36" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="J36" s="44"/>
+      <c r="J36" s="44" t="s">
+        <v>136</v>
+      </c>
       <c r="K36" s="44"/>
       <c r="L36" s="44"/>
       <c r="M36" s="44"/>
@@ -4183,9 +4297,9 @@
       <c r="R36" s="45"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="173"/>
-      <c r="B37" s="174"/>
-      <c r="C37" s="174"/>
+      <c r="A37" s="177"/>
+      <c r="B37" s="178"/>
+      <c r="C37" s="178"/>
       <c r="D37" s="134" t="s">
         <v>22</v>
       </c>
@@ -4196,7 +4310,9 @@
       <c r="I37" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="J37" s="56"/>
+      <c r="J37" s="56" t="s">
+        <v>86</v>
+      </c>
       <c r="K37" s="56"/>
       <c r="L37" s="56"/>
       <c r="M37" s="56"/>
@@ -4207,13 +4323,13 @@
       <c r="R37" s="57"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="176" t="s">
+      <c r="A38" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="177" t="s">
+      <c r="B38" s="181" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="178" t="s">
+      <c r="C38" s="182" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="135" t="s">
@@ -4226,7 +4342,9 @@
       <c r="I38" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J38" s="46"/>
+      <c r="J38" s="46" t="s">
+        <v>87</v>
+      </c>
       <c r="K38" s="46"/>
       <c r="L38" s="46"/>
       <c r="M38" s="46"/>
@@ -4237,9 +4355,9 @@
       <c r="R38" s="47"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="176"/>
-      <c r="B39" s="177"/>
-      <c r="C39" s="178"/>
+      <c r="A39" s="180"/>
+      <c r="B39" s="181"/>
+      <c r="C39" s="182"/>
       <c r="D39" s="136" t="s">
         <v>19</v>
       </c>
@@ -4250,7 +4368,9 @@
       <c r="I39" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="J39" s="48"/>
+      <c r="J39" s="48" t="s">
+        <v>137</v>
+      </c>
       <c r="K39" s="48"/>
       <c r="L39" s="48"/>
       <c r="M39" s="48"/>
@@ -4261,9 +4381,9 @@
       <c r="R39" s="49"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="176"/>
-      <c r="B40" s="177"/>
-      <c r="C40" s="178"/>
+      <c r="A40" s="180"/>
+      <c r="B40" s="181"/>
+      <c r="C40" s="182"/>
       <c r="D40" s="136" t="s">
         <v>21</v>
       </c>
@@ -4274,7 +4394,9 @@
       <c r="I40" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="48"/>
+      <c r="J40" s="48" t="s">
+        <v>138</v>
+      </c>
       <c r="K40" s="48"/>
       <c r="L40" s="48"/>
       <c r="M40" s="48"/>
@@ -4285,9 +4407,9 @@
       <c r="R40" s="49"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="176"/>
-      <c r="B41" s="177"/>
-      <c r="C41" s="177"/>
+      <c r="A41" s="180"/>
+      <c r="B41" s="181"/>
+      <c r="C41" s="181"/>
       <c r="D41" s="137" t="s">
         <v>22</v>
       </c>
@@ -4298,7 +4420,9 @@
       <c r="I41" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="J41" s="58"/>
+      <c r="J41" s="58" t="s">
+        <v>88</v>
+      </c>
       <c r="K41" s="58"/>
       <c r="L41" s="58"/>
       <c r="M41" s="58"/>
@@ -4309,13 +4433,13 @@
       <c r="R41" s="59"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="179" t="s">
+      <c r="A42" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="181" t="s">
+      <c r="B42" s="170" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="182" t="s">
+      <c r="C42" s="171" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="138" t="s">
@@ -4328,7 +4452,9 @@
       <c r="I42" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="J42" s="50"/>
+      <c r="J42" s="50" t="s">
+        <v>139</v>
+      </c>
       <c r="K42" s="50"/>
       <c r="L42" s="50"/>
       <c r="M42" s="50"/>
@@ -4339,9 +4465,9 @@
       <c r="R42" s="51"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="179"/>
-      <c r="B43" s="181"/>
-      <c r="C43" s="182"/>
+      <c r="A43" s="168"/>
+      <c r="B43" s="170"/>
+      <c r="C43" s="171"/>
       <c r="D43" s="139" t="s">
         <v>19</v>
       </c>
@@ -4352,7 +4478,9 @@
       <c r="I43" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="J43" s="52"/>
+      <c r="J43" s="52" t="s">
+        <v>140</v>
+      </c>
       <c r="K43" s="52"/>
       <c r="L43" s="52"/>
       <c r="M43" s="52"/>
@@ -4363,9 +4491,9 @@
       <c r="R43" s="53"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="179"/>
-      <c r="B44" s="181"/>
-      <c r="C44" s="182"/>
+      <c r="A44" s="168"/>
+      <c r="B44" s="170"/>
+      <c r="C44" s="171"/>
       <c r="D44" s="139" t="s">
         <v>21</v>
       </c>
@@ -4376,7 +4504,9 @@
       <c r="I44" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="J44" s="52"/>
+      <c r="J44" s="52" t="s">
+        <v>141</v>
+      </c>
       <c r="K44" s="52"/>
       <c r="L44" s="52"/>
       <c r="M44" s="52"/>
@@ -4387,9 +4517,9 @@
       <c r="R44" s="53"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="180"/>
-      <c r="B45" s="181"/>
-      <c r="C45" s="181"/>
+      <c r="A45" s="169"/>
+      <c r="B45" s="170"/>
+      <c r="C45" s="170"/>
       <c r="D45" s="139" t="s">
         <v>22</v>
       </c>
@@ -4400,7 +4530,9 @@
       <c r="I45" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="J45" s="52"/>
+      <c r="J45" s="52" t="s">
+        <v>142</v>
+      </c>
       <c r="K45" s="52"/>
       <c r="L45" s="52"/>
       <c r="M45" s="52"/>
@@ -4411,56 +4543,58 @@
       <c r="R45" s="53"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="183" t="s">
+      <c r="A46" s="172" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="184"/>
-      <c r="C46" s="184"/>
-      <c r="D46" s="185"/>
-      <c r="E46" s="186"/>
-      <c r="F46" s="188"/>
-      <c r="G46" s="188"/>
-      <c r="H46" s="188"/>
-      <c r="I46" s="192" t="s">
+      <c r="B46" s="173"/>
+      <c r="C46" s="173"/>
+      <c r="D46" s="174"/>
+      <c r="E46" s="175"/>
+      <c r="F46" s="147"/>
+      <c r="G46" s="147"/>
+      <c r="H46" s="147"/>
+      <c r="I46" s="166" t="s">
         <v>1</v>
       </c>
-      <c r="J46" s="188"/>
-      <c r="K46" s="188"/>
-      <c r="L46" s="188"/>
-      <c r="M46" s="188"/>
-      <c r="N46" s="188"/>
-      <c r="O46" s="188"/>
-      <c r="P46" s="188"/>
-      <c r="Q46" s="188"/>
-      <c r="R46" s="190"/>
+      <c r="J46" s="166" t="s">
+        <v>132</v>
+      </c>
+      <c r="K46" s="147"/>
+      <c r="L46" s="147"/>
+      <c r="M46" s="147"/>
+      <c r="N46" s="147"/>
+      <c r="O46" s="147"/>
+      <c r="P46" s="147"/>
+      <c r="Q46" s="147"/>
+      <c r="R46" s="164"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="183"/>
-      <c r="B47" s="184"/>
-      <c r="C47" s="184"/>
-      <c r="D47" s="185"/>
-      <c r="E47" s="187"/>
-      <c r="F47" s="189"/>
-      <c r="G47" s="189"/>
-      <c r="H47" s="189"/>
-      <c r="I47" s="193"/>
-      <c r="J47" s="189"/>
-      <c r="K47" s="189"/>
-      <c r="L47" s="189"/>
-      <c r="M47" s="189"/>
-      <c r="N47" s="189"/>
-      <c r="O47" s="189"/>
-      <c r="P47" s="189"/>
-      <c r="Q47" s="189"/>
-      <c r="R47" s="191"/>
+      <c r="A47" s="172"/>
+      <c r="B47" s="173"/>
+      <c r="C47" s="173"/>
+      <c r="D47" s="174"/>
+      <c r="E47" s="176"/>
+      <c r="F47" s="148"/>
+      <c r="G47" s="148"/>
+      <c r="H47" s="148"/>
+      <c r="I47" s="167"/>
+      <c r="J47" s="167"/>
+      <c r="K47" s="148"/>
+      <c r="L47" s="148"/>
+      <c r="M47" s="148"/>
+      <c r="N47" s="148"/>
+      <c r="O47" s="148"/>
+      <c r="P47" s="148"/>
+      <c r="Q47" s="148"/>
+      <c r="R47" s="165"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="197" t="s">
+      <c r="A48" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="198"/>
-      <c r="C48" s="198"/>
-      <c r="D48" s="199"/>
+      <c r="B48" s="150"/>
+      <c r="C48" s="150"/>
+      <c r="D48" s="151"/>
       <c r="E48" s="104"/>
       <c r="F48" s="65"/>
       <c r="G48" s="65"/>
@@ -4468,7 +4602,9 @@
       <c r="I48" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="J48" s="65"/>
+      <c r="J48" s="65" t="s">
+        <v>36</v>
+      </c>
       <c r="K48" s="65"/>
       <c r="L48" s="65"/>
       <c r="M48" s="65"/>
@@ -4479,12 +4615,12 @@
       <c r="R48" s="66"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="200" t="s">
+      <c r="A49" s="152" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="201"/>
-      <c r="C49" s="201"/>
-      <c r="D49" s="202"/>
+      <c r="B49" s="153"/>
+      <c r="C49" s="153"/>
+      <c r="D49" s="154"/>
       <c r="E49" s="105"/>
       <c r="F49" s="63"/>
       <c r="G49" s="63"/>
@@ -4492,7 +4628,9 @@
       <c r="I49" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="J49" s="63"/>
+      <c r="J49" s="63" t="s">
+        <v>143</v>
+      </c>
       <c r="K49" s="63"/>
       <c r="L49" s="63"/>
       <c r="M49" s="63"/>
@@ -4503,12 +4641,12 @@
       <c r="R49" s="64"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="203" t="s">
+      <c r="A50" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="204"/>
-      <c r="C50" s="204"/>
-      <c r="D50" s="205"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="156"/>
+      <c r="D50" s="157"/>
       <c r="E50" s="106"/>
       <c r="F50" s="67"/>
       <c r="G50" s="67"/>
@@ -4516,7 +4654,9 @@
       <c r="I50" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="J50" s="67"/>
+      <c r="J50" s="67" t="s">
+        <v>144</v>
+      </c>
       <c r="K50" s="67"/>
       <c r="L50" s="67"/>
       <c r="M50" s="67"/>
@@ -4527,12 +4667,12 @@
       <c r="R50" s="68"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="206" t="s">
+      <c r="A51" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="207"/>
-      <c r="C51" s="207"/>
-      <c r="D51" s="208"/>
+      <c r="B51" s="159"/>
+      <c r="C51" s="159"/>
+      <c r="D51" s="160"/>
       <c r="E51" s="107"/>
       <c r="F51" s="69"/>
       <c r="G51" s="69"/>
@@ -4540,7 +4680,9 @@
       <c r="I51" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="J51" s="69"/>
+      <c r="J51" s="69" t="s">
+        <v>145</v>
+      </c>
       <c r="K51" s="69"/>
       <c r="L51" s="69"/>
       <c r="M51" s="69"/>
@@ -4551,12 +4693,12 @@
       <c r="R51" s="70"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="209" t="s">
+      <c r="A52" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="210"/>
-      <c r="C52" s="210"/>
-      <c r="D52" s="211"/>
+      <c r="B52" s="162"/>
+      <c r="C52" s="162"/>
+      <c r="D52" s="163"/>
       <c r="E52" s="108"/>
       <c r="F52" s="71"/>
       <c r="G52" s="71"/>
@@ -4564,7 +4706,9 @@
       <c r="I52" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="J52" s="71"/>
+      <c r="J52" s="71" t="s">
+        <v>146</v>
+      </c>
       <c r="K52" s="71"/>
       <c r="L52" s="71"/>
       <c r="M52" s="71"/>
@@ -4575,12 +4719,12 @@
       <c r="R52" s="72"/>
     </row>
     <row r="53" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="194" t="s">
+      <c r="A53" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="195"/>
-      <c r="C53" s="195"/>
-      <c r="D53" s="196"/>
+      <c r="B53" s="145"/>
+      <c r="C53" s="145"/>
+      <c r="D53" s="146"/>
       <c r="E53" s="109"/>
       <c r="F53" s="73"/>
       <c r="G53" s="73"/>
@@ -4588,7 +4732,9 @@
       <c r="I53" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="J53" s="73"/>
+      <c r="J53" s="73" t="s">
+        <v>147</v>
+      </c>
       <c r="K53" s="73"/>
       <c r="L53" s="73"/>
       <c r="M53" s="73"/>
@@ -4601,6 +4747,51 @@
     <row r="54" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="A2:D4"/>
+    <mergeCell ref="E2:R3"/>
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="A46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="Q46:Q47"/>
+    <mergeCell ref="R46:R47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="H46:H47"/>
+    <mergeCell ref="I46:I47"/>
+    <mergeCell ref="J46:J47"/>
+    <mergeCell ref="K46:K47"/>
+    <mergeCell ref="L46:L47"/>
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="M46:M47"/>
     <mergeCell ref="N46:N47"/>
@@ -4612,51 +4803,6 @@
     <mergeCell ref="A50:D50"/>
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A52:D52"/>
-    <mergeCell ref="Q46:Q47"/>
-    <mergeCell ref="R46:R47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="H46:H47"/>
-    <mergeCell ref="I46:I47"/>
-    <mergeCell ref="J46:J47"/>
-    <mergeCell ref="K46:K47"/>
-    <mergeCell ref="L46:L47"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="A46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:R1"/>
-    <mergeCell ref="A2:D4"/>
-    <mergeCell ref="E2:R3"/>
-    <mergeCell ref="E4:R4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4678,94 +4824,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="37.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="197" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146" t="s">
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="198" t="s">
         <v>100</v>
       </c>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
-      <c r="O1" s="146"/>
-      <c r="P1" s="146"/>
-      <c r="Q1" s="146"/>
-      <c r="R1" s="147"/>
+      <c r="K1" s="198"/>
+      <c r="L1" s="198"/>
+      <c r="M1" s="198"/>
+      <c r="N1" s="198"/>
+      <c r="O1" s="198"/>
+      <c r="P1" s="198"/>
+      <c r="Q1" s="198"/>
+      <c r="R1" s="199"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="200" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="154" t="s">
+      <c r="B2" s="201"/>
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
+      <c r="E2" s="206" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="154"/>
-      <c r="P2" s="154"/>
-      <c r="Q2" s="154"/>
-      <c r="R2" s="155"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="206"/>
+      <c r="I2" s="206"/>
+      <c r="J2" s="206"/>
+      <c r="K2" s="206"/>
+      <c r="L2" s="206"/>
+      <c r="M2" s="206"/>
+      <c r="N2" s="206"/>
+      <c r="O2" s="206"/>
+      <c r="P2" s="206"/>
+      <c r="Q2" s="206"/>
+      <c r="R2" s="207"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="150"/>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
-      <c r="M3" s="156"/>
-      <c r="N3" s="156"/>
-      <c r="O3" s="156"/>
-      <c r="P3" s="156"/>
-      <c r="Q3" s="156"/>
-      <c r="R3" s="157"/>
+      <c r="A3" s="202"/>
+      <c r="B3" s="203"/>
+      <c r="C3" s="203"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="208"/>
+      <c r="F3" s="208"/>
+      <c r="G3" s="208"/>
+      <c r="H3" s="208"/>
+      <c r="I3" s="208"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="208"/>
+      <c r="L3" s="208"/>
+      <c r="M3" s="208"/>
+      <c r="N3" s="208"/>
+      <c r="O3" s="208"/>
+      <c r="P3" s="208"/>
+      <c r="Q3" s="208"/>
+      <c r="R3" s="209"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="152"/>
-      <c r="B4" s="153"/>
-      <c r="C4" s="153"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="158" t="s">
+      <c r="A4" s="204"/>
+      <c r="B4" s="205"/>
+      <c r="C4" s="205"/>
+      <c r="D4" s="205"/>
+      <c r="E4" s="210" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="159"/>
-      <c r="G4" s="159"/>
-      <c r="H4" s="159"/>
-      <c r="I4" s="159"/>
-      <c r="J4" s="159"/>
-      <c r="K4" s="159"/>
-      <c r="L4" s="159"/>
-      <c r="M4" s="159"/>
-      <c r="N4" s="159"/>
-      <c r="O4" s="159"/>
-      <c r="P4" s="159"/>
-      <c r="Q4" s="159"/>
-      <c r="R4" s="160"/>
+      <c r="F4" s="211"/>
+      <c r="G4" s="211"/>
+      <c r="H4" s="211"/>
+      <c r="I4" s="211"/>
+      <c r="J4" s="211"/>
+      <c r="K4" s="211"/>
+      <c r="L4" s="211"/>
+      <c r="M4" s="211"/>
+      <c r="N4" s="211"/>
+      <c r="O4" s="211"/>
+      <c r="P4" s="211"/>
+      <c r="Q4" s="211"/>
+      <c r="R4" s="212"/>
     </row>
     <row r="5" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
@@ -4798,13 +4944,13 @@
       <c r="R5" s="142"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="143" t="s">
+      <c r="A6" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="144">
+      <c r="C6" s="196">
         <v>8</v>
       </c>
       <c r="D6" s="111" t="s">
@@ -4828,9 +4974,9 @@
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="143"/>
-      <c r="B7" s="144"/>
-      <c r="C7" s="144"/>
+      <c r="A7" s="195"/>
+      <c r="B7" s="196"/>
+      <c r="C7" s="196"/>
       <c r="D7" s="112" t="s">
         <v>19</v>
       </c>
@@ -4852,9 +4998,9 @@
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="143"/>
-      <c r="B8" s="144"/>
-      <c r="C8" s="144"/>
+      <c r="A8" s="195"/>
+      <c r="B8" s="196"/>
+      <c r="C8" s="196"/>
       <c r="D8" s="112" t="s">
         <v>21</v>
       </c>
@@ -4876,9 +5022,9 @@
       <c r="R8" s="5"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="143"/>
-      <c r="B9" s="144"/>
-      <c r="C9" s="144"/>
+      <c r="A9" s="195"/>
+      <c r="B9" s="196"/>
+      <c r="C9" s="196"/>
       <c r="D9" s="113" t="s">
         <v>22</v>
       </c>
@@ -4900,13 +5046,13 @@
       <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="161" t="s">
+      <c r="A10" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="162" t="s">
+      <c r="B10" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="162">
+      <c r="C10" s="192">
         <v>8</v>
       </c>
       <c r="D10" s="114" t="s">
@@ -4930,9 +5076,9 @@
       <c r="R10" s="9"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="161"/>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
+      <c r="A11" s="191"/>
+      <c r="B11" s="192"/>
+      <c r="C11" s="192"/>
       <c r="D11" s="115" t="s">
         <v>19</v>
       </c>
@@ -4954,9 +5100,9 @@
       <c r="R11" s="11"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="161"/>
-      <c r="B12" s="162"/>
-      <c r="C12" s="162"/>
+      <c r="A12" s="191"/>
+      <c r="B12" s="192"/>
+      <c r="C12" s="192"/>
       <c r="D12" s="115" t="s">
         <v>21</v>
       </c>
@@ -4978,9 +5124,9 @@
       <c r="R12" s="11"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="161"/>
-      <c r="B13" s="162"/>
-      <c r="C13" s="162"/>
+      <c r="A13" s="191"/>
+      <c r="B13" s="192"/>
+      <c r="C13" s="192"/>
       <c r="D13" s="116" t="s">
         <v>22</v>
       </c>
@@ -5002,13 +5148,13 @@
       <c r="R13" s="13"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="163" t="s">
+      <c r="A14" s="193" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="164">
+      <c r="C14" s="194">
         <v>16</v>
       </c>
       <c r="D14" s="117" t="s">
@@ -5032,9 +5178,9 @@
       <c r="R14" s="15"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="163"/>
-      <c r="B15" s="164"/>
-      <c r="C15" s="164"/>
+      <c r="A15" s="193"/>
+      <c r="B15" s="194"/>
+      <c r="C15" s="194"/>
       <c r="D15" s="118" t="s">
         <v>19</v>
       </c>
@@ -5056,9 +5202,9 @@
       <c r="R15" s="17"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="163"/>
-      <c r="B16" s="164"/>
-      <c r="C16" s="164"/>
+      <c r="A16" s="193"/>
+      <c r="B16" s="194"/>
+      <c r="C16" s="194"/>
       <c r="D16" s="118" t="s">
         <v>21</v>
       </c>
@@ -5080,9 +5226,9 @@
       <c r="R16" s="17"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="163"/>
-      <c r="B17" s="164"/>
-      <c r="C17" s="164"/>
+      <c r="A17" s="193"/>
+      <c r="B17" s="194"/>
+      <c r="C17" s="194"/>
       <c r="D17" s="119" t="s">
         <v>22</v>
       </c>
@@ -5104,13 +5250,13 @@
       <c r="R17" s="19"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="165" t="s">
+      <c r="A18" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="166" t="s">
+      <c r="B18" s="188" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="166">
+      <c r="C18" s="188">
         <v>16</v>
       </c>
       <c r="D18" s="120" t="s">
@@ -5134,9 +5280,9 @@
       <c r="R18" s="21"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="165"/>
-      <c r="B19" s="166"/>
-      <c r="C19" s="166"/>
+      <c r="A19" s="187"/>
+      <c r="B19" s="188"/>
+      <c r="C19" s="188"/>
       <c r="D19" s="121" t="s">
         <v>19</v>
       </c>
@@ -5158,9 +5304,9 @@
       <c r="R19" s="23"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="165"/>
-      <c r="B20" s="166"/>
-      <c r="C20" s="166"/>
+      <c r="A20" s="187"/>
+      <c r="B20" s="188"/>
+      <c r="C20" s="188"/>
       <c r="D20" s="121" t="s">
         <v>21</v>
       </c>
@@ -5182,9 +5328,9 @@
       <c r="R20" s="23"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="165"/>
-      <c r="B21" s="166"/>
-      <c r="C21" s="166"/>
+      <c r="A21" s="187"/>
+      <c r="B21" s="188"/>
+      <c r="C21" s="188"/>
       <c r="D21" s="122" t="s">
         <v>22</v>
       </c>
@@ -5206,13 +5352,13 @@
       <c r="R21" s="25"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="167" t="s">
+      <c r="A22" s="189" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="168" t="s">
+      <c r="B22" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="168">
+      <c r="C22" s="190">
         <v>32</v>
       </c>
       <c r="D22" s="123" t="s">
@@ -5236,9 +5382,9 @@
       <c r="R22" s="27"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="167"/>
-      <c r="B23" s="168"/>
-      <c r="C23" s="168"/>
+      <c r="A23" s="189"/>
+      <c r="B23" s="190"/>
+      <c r="C23" s="190"/>
       <c r="D23" s="124" t="s">
         <v>19</v>
       </c>
@@ -5260,9 +5406,9 @@
       <c r="R23" s="29"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="167"/>
-      <c r="B24" s="168"/>
-      <c r="C24" s="168"/>
+      <c r="A24" s="189"/>
+      <c r="B24" s="190"/>
+      <c r="C24" s="190"/>
       <c r="D24" s="124" t="s">
         <v>21</v>
       </c>
@@ -5284,9 +5430,9 @@
       <c r="R24" s="29"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="167"/>
-      <c r="B25" s="168"/>
-      <c r="C25" s="168"/>
+      <c r="A25" s="189"/>
+      <c r="B25" s="190"/>
+      <c r="C25" s="190"/>
       <c r="D25" s="125" t="s">
         <v>22</v>
       </c>
@@ -5308,13 +5454,13 @@
       <c r="R25" s="31"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="169" t="s">
+      <c r="A26" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="170" t="s">
+      <c r="B26" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="170">
+      <c r="C26" s="184">
         <v>32</v>
       </c>
       <c r="D26" s="126" t="s">
@@ -5338,9 +5484,9 @@
       <c r="R26" s="33"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="169"/>
-      <c r="B27" s="170"/>
-      <c r="C27" s="170"/>
+      <c r="A27" s="183"/>
+      <c r="B27" s="184"/>
+      <c r="C27" s="184"/>
       <c r="D27" s="127" t="s">
         <v>19</v>
       </c>
@@ -5362,9 +5508,9 @@
       <c r="R27" s="35"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="169"/>
-      <c r="B28" s="170"/>
-      <c r="C28" s="170"/>
+      <c r="A28" s="183"/>
+      <c r="B28" s="184"/>
+      <c r="C28" s="184"/>
       <c r="D28" s="127" t="s">
         <v>21</v>
       </c>
@@ -5386,9 +5532,9 @@
       <c r="R28" s="35"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="169"/>
-      <c r="B29" s="170"/>
-      <c r="C29" s="170"/>
+      <c r="A29" s="183"/>
+      <c r="B29" s="184"/>
+      <c r="C29" s="184"/>
       <c r="D29" s="128" t="s">
         <v>22</v>
       </c>
@@ -5410,13 +5556,13 @@
       <c r="R29" s="37"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="171" t="s">
+      <c r="A30" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="172" t="s">
+      <c r="B30" s="186" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="172">
+      <c r="C30" s="186">
         <v>32</v>
       </c>
       <c r="D30" s="129" t="s">
@@ -5440,9 +5586,9 @@
       <c r="R30" s="39"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="171"/>
-      <c r="B31" s="172"/>
-      <c r="C31" s="172"/>
+      <c r="A31" s="185"/>
+      <c r="B31" s="186"/>
+      <c r="C31" s="186"/>
       <c r="D31" s="130" t="s">
         <v>19</v>
       </c>
@@ -5464,9 +5610,9 @@
       <c r="R31" s="41"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="171"/>
-      <c r="B32" s="172"/>
-      <c r="C32" s="172"/>
+      <c r="A32" s="185"/>
+      <c r="B32" s="186"/>
+      <c r="C32" s="186"/>
       <c r="D32" s="130" t="s">
         <v>21</v>
       </c>
@@ -5488,9 +5634,9 @@
       <c r="R32" s="41"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="171"/>
-      <c r="B33" s="172"/>
-      <c r="C33" s="172"/>
+      <c r="A33" s="185"/>
+      <c r="B33" s="186"/>
+      <c r="C33" s="186"/>
       <c r="D33" s="131" t="s">
         <v>22</v>
       </c>
@@ -5512,13 +5658,13 @@
       <c r="R33" s="55"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="173" t="s">
+      <c r="A34" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="174" t="s">
+      <c r="B34" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="175" t="s">
+      <c r="C34" s="179" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="132" t="s">
@@ -5542,9 +5688,9 @@
       <c r="R34" s="43"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="173"/>
-      <c r="B35" s="174"/>
-      <c r="C35" s="175"/>
+      <c r="A35" s="177"/>
+      <c r="B35" s="178"/>
+      <c r="C35" s="179"/>
       <c r="D35" s="133" t="s">
         <v>19</v>
       </c>
@@ -5566,9 +5712,9 @@
       <c r="R35" s="45"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="173"/>
-      <c r="B36" s="174"/>
-      <c r="C36" s="175"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="178"/>
+      <c r="C36" s="179"/>
       <c r="D36" s="133" t="s">
         <v>21</v>
       </c>
@@ -5590,9 +5736,9 @@
       <c r="R36" s="45"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="173"/>
-      <c r="B37" s="174"/>
-      <c r="C37" s="174"/>
+      <c r="A37" s="177"/>
+      <c r="B37" s="178"/>
+      <c r="C37" s="178"/>
       <c r="D37" s="134" t="s">
         <v>22</v>
       </c>
@@ -5614,13 +5760,13 @@
       <c r="R37" s="57"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="176" t="s">
+      <c r="A38" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="177" t="s">
+      <c r="B38" s="181" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="178" t="s">
+      <c r="C38" s="182" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="135" t="s">
@@ -5644,9 +5790,9 @@
       <c r="R38" s="47"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="176"/>
-      <c r="B39" s="177"/>
-      <c r="C39" s="178"/>
+      <c r="A39" s="180"/>
+      <c r="B39" s="181"/>
+      <c r="C39" s="182"/>
       <c r="D39" s="136" t="s">
         <v>19</v>
       </c>
@@ -5668,9 +5814,9 @@
       <c r="R39" s="49"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="176"/>
-      <c r="B40" s="177"/>
-      <c r="C40" s="178"/>
+      <c r="A40" s="180"/>
+      <c r="B40" s="181"/>
+      <c r="C40" s="182"/>
       <c r="D40" s="136" t="s">
         <v>21</v>
       </c>
@@ -5692,9 +5838,9 @@
       <c r="R40" s="49"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="176"/>
-      <c r="B41" s="177"/>
-      <c r="C41" s="177"/>
+      <c r="A41" s="180"/>
+      <c r="B41" s="181"/>
+      <c r="C41" s="181"/>
       <c r="D41" s="137" t="s">
         <v>22</v>
       </c>
@@ -5716,13 +5862,13 @@
       <c r="R41" s="59"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="179" t="s">
+      <c r="A42" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="181" t="s">
+      <c r="B42" s="170" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="182">
+      <c r="C42" s="171">
         <v>2048</v>
       </c>
       <c r="D42" s="138" t="s">
@@ -5746,9 +5892,9 @@
       <c r="R42" s="51"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="179"/>
-      <c r="B43" s="181"/>
-      <c r="C43" s="182"/>
+      <c r="A43" s="168"/>
+      <c r="B43" s="170"/>
+      <c r="C43" s="171"/>
       <c r="D43" s="139" t="s">
         <v>19</v>
       </c>
@@ -5770,9 +5916,9 @@
       <c r="R43" s="53"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="179"/>
-      <c r="B44" s="181"/>
-      <c r="C44" s="182"/>
+      <c r="A44" s="168"/>
+      <c r="B44" s="170"/>
+      <c r="C44" s="171"/>
       <c r="D44" s="139" t="s">
         <v>21</v>
       </c>
@@ -5794,9 +5940,9 @@
       <c r="R44" s="53"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="180"/>
-      <c r="B45" s="181"/>
-      <c r="C45" s="181"/>
+      <c r="A45" s="169"/>
+      <c r="B45" s="170"/>
+      <c r="C45" s="170"/>
       <c r="D45" s="139" t="s">
         <v>22</v>
       </c>
@@ -5818,56 +5964,56 @@
       <c r="R45" s="53"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="183" t="s">
+      <c r="A46" s="172" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="184"/>
-      <c r="C46" s="184"/>
-      <c r="D46" s="185"/>
-      <c r="E46" s="186"/>
-      <c r="F46" s="188"/>
-      <c r="G46" s="188"/>
-      <c r="H46" s="188"/>
-      <c r="I46" s="192" t="s">
+      <c r="B46" s="173"/>
+      <c r="C46" s="173"/>
+      <c r="D46" s="174"/>
+      <c r="E46" s="175"/>
+      <c r="F46" s="147"/>
+      <c r="G46" s="147"/>
+      <c r="H46" s="147"/>
+      <c r="I46" s="166" t="s">
         <v>1</v>
       </c>
-      <c r="J46" s="188"/>
-      <c r="K46" s="188"/>
-      <c r="L46" s="188"/>
-      <c r="M46" s="188"/>
-      <c r="N46" s="188"/>
-      <c r="O46" s="188"/>
-      <c r="P46" s="188"/>
-      <c r="Q46" s="188"/>
-      <c r="R46" s="190"/>
+      <c r="J46" s="147"/>
+      <c r="K46" s="147"/>
+      <c r="L46" s="147"/>
+      <c r="M46" s="147"/>
+      <c r="N46" s="147"/>
+      <c r="O46" s="147"/>
+      <c r="P46" s="147"/>
+      <c r="Q46" s="147"/>
+      <c r="R46" s="164"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="183"/>
-      <c r="B47" s="184"/>
-      <c r="C47" s="184"/>
-      <c r="D47" s="185"/>
-      <c r="E47" s="187"/>
-      <c r="F47" s="189"/>
-      <c r="G47" s="189"/>
-      <c r="H47" s="189"/>
-      <c r="I47" s="193"/>
-      <c r="J47" s="189"/>
-      <c r="K47" s="189"/>
-      <c r="L47" s="189"/>
-      <c r="M47" s="189"/>
-      <c r="N47" s="189"/>
-      <c r="O47" s="189"/>
-      <c r="P47" s="189"/>
-      <c r="Q47" s="189"/>
-      <c r="R47" s="191"/>
+      <c r="A47" s="172"/>
+      <c r="B47" s="173"/>
+      <c r="C47" s="173"/>
+      <c r="D47" s="174"/>
+      <c r="E47" s="176"/>
+      <c r="F47" s="148"/>
+      <c r="G47" s="148"/>
+      <c r="H47" s="148"/>
+      <c r="I47" s="167"/>
+      <c r="J47" s="148"/>
+      <c r="K47" s="148"/>
+      <c r="L47" s="148"/>
+      <c r="M47" s="148"/>
+      <c r="N47" s="148"/>
+      <c r="O47" s="148"/>
+      <c r="P47" s="148"/>
+      <c r="Q47" s="148"/>
+      <c r="R47" s="165"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="197" t="s">
+      <c r="A48" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="198"/>
-      <c r="C48" s="198"/>
-      <c r="D48" s="199"/>
+      <c r="B48" s="150"/>
+      <c r="C48" s="150"/>
+      <c r="D48" s="151"/>
       <c r="E48" s="104"/>
       <c r="F48" s="65"/>
       <c r="G48" s="65"/>
@@ -5886,12 +6032,12 @@
       <c r="R48" s="66"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="200" t="s">
+      <c r="A49" s="152" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="201"/>
-      <c r="C49" s="201"/>
-      <c r="D49" s="202"/>
+      <c r="B49" s="153"/>
+      <c r="C49" s="153"/>
+      <c r="D49" s="154"/>
       <c r="E49" s="105"/>
       <c r="F49" s="63"/>
       <c r="G49" s="63"/>
@@ -5910,12 +6056,12 @@
       <c r="R49" s="64"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="203" t="s">
+      <c r="A50" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="204"/>
-      <c r="C50" s="204"/>
-      <c r="D50" s="205"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="156"/>
+      <c r="D50" s="157"/>
       <c r="E50" s="106"/>
       <c r="F50" s="67"/>
       <c r="G50" s="67"/>
@@ -5934,12 +6080,12 @@
       <c r="R50" s="68"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="206" t="s">
+      <c r="A51" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="207"/>
-      <c r="C51" s="207"/>
-      <c r="D51" s="208"/>
+      <c r="B51" s="159"/>
+      <c r="C51" s="159"/>
+      <c r="D51" s="160"/>
       <c r="E51" s="107"/>
       <c r="F51" s="69"/>
       <c r="G51" s="69"/>
@@ -5958,12 +6104,12 @@
       <c r="R51" s="70"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="209" t="s">
+      <c r="A52" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="210"/>
-      <c r="C52" s="210"/>
-      <c r="D52" s="211"/>
+      <c r="B52" s="162"/>
+      <c r="C52" s="162"/>
+      <c r="D52" s="163"/>
       <c r="E52" s="108"/>
       <c r="F52" s="71"/>
       <c r="G52" s="71"/>
@@ -5982,12 +6128,12 @@
       <c r="R52" s="72"/>
     </row>
     <row r="53" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="194" t="s">
+      <c r="A53" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="195"/>
-      <c r="C53" s="195"/>
-      <c r="D53" s="196"/>
+      <c r="B53" s="145"/>
+      <c r="C53" s="145"/>
+      <c r="D53" s="146"/>
       <c r="E53" s="109"/>
       <c r="F53" s="73"/>
       <c r="G53" s="73"/>
@@ -6008,6 +6154,49 @@
     <row r="54" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="A2:D4"/>
+    <mergeCell ref="E2:R3"/>
+    <mergeCell ref="E4:R4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="Q46:Q47"/>
+    <mergeCell ref="R46:R47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="H46:H47"/>
+    <mergeCell ref="I46:I47"/>
+    <mergeCell ref="J46:J47"/>
+    <mergeCell ref="K46:K47"/>
+    <mergeCell ref="L46:L47"/>
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="M46:M47"/>
     <mergeCell ref="N46:N47"/>
@@ -6021,49 +6210,6 @@
     <mergeCell ref="A52:D52"/>
     <mergeCell ref="A46:D47"/>
     <mergeCell ref="E46:E47"/>
-    <mergeCell ref="Q46:Q47"/>
-    <mergeCell ref="R46:R47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="H46:H47"/>
-    <mergeCell ref="I46:I47"/>
-    <mergeCell ref="J46:J47"/>
-    <mergeCell ref="K46:K47"/>
-    <mergeCell ref="L46:L47"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:R1"/>
-    <mergeCell ref="A2:D4"/>
-    <mergeCell ref="E2:R3"/>
-    <mergeCell ref="E4:R4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6084,94 +6230,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="37.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="197" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146" t="s">
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="198" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
-      <c r="O1" s="146"/>
-      <c r="P1" s="146"/>
-      <c r="Q1" s="146"/>
-      <c r="R1" s="147"/>
+      <c r="K1" s="198"/>
+      <c r="L1" s="198"/>
+      <c r="M1" s="198"/>
+      <c r="N1" s="198"/>
+      <c r="O1" s="198"/>
+      <c r="P1" s="198"/>
+      <c r="Q1" s="198"/>
+      <c r="R1" s="199"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="200" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="154" t="s">
+      <c r="B2" s="201"/>
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
+      <c r="E2" s="206" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="154"/>
-      <c r="P2" s="154"/>
-      <c r="Q2" s="154"/>
-      <c r="R2" s="155"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="206"/>
+      <c r="I2" s="206"/>
+      <c r="J2" s="206"/>
+      <c r="K2" s="206"/>
+      <c r="L2" s="206"/>
+      <c r="M2" s="206"/>
+      <c r="N2" s="206"/>
+      <c r="O2" s="206"/>
+      <c r="P2" s="206"/>
+      <c r="Q2" s="206"/>
+      <c r="R2" s="207"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="150"/>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
-      <c r="M3" s="156"/>
-      <c r="N3" s="156"/>
-      <c r="O3" s="156"/>
-      <c r="P3" s="156"/>
-      <c r="Q3" s="156"/>
-      <c r="R3" s="157"/>
+      <c r="A3" s="202"/>
+      <c r="B3" s="203"/>
+      <c r="C3" s="203"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="208"/>
+      <c r="F3" s="208"/>
+      <c r="G3" s="208"/>
+      <c r="H3" s="208"/>
+      <c r="I3" s="208"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="208"/>
+      <c r="L3" s="208"/>
+      <c r="M3" s="208"/>
+      <c r="N3" s="208"/>
+      <c r="O3" s="208"/>
+      <c r="P3" s="208"/>
+      <c r="Q3" s="208"/>
+      <c r="R3" s="209"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="152"/>
-      <c r="B4" s="153"/>
-      <c r="C4" s="153"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="158" t="s">
+      <c r="A4" s="204"/>
+      <c r="B4" s="205"/>
+      <c r="C4" s="205"/>
+      <c r="D4" s="205"/>
+      <c r="E4" s="210" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="159"/>
-      <c r="G4" s="159"/>
-      <c r="H4" s="159"/>
-      <c r="I4" s="159"/>
-      <c r="J4" s="159"/>
-      <c r="K4" s="159"/>
-      <c r="L4" s="159"/>
-      <c r="M4" s="159"/>
-      <c r="N4" s="159"/>
-      <c r="O4" s="159"/>
-      <c r="P4" s="159"/>
-      <c r="Q4" s="159"/>
-      <c r="R4" s="160"/>
+      <c r="F4" s="211"/>
+      <c r="G4" s="211"/>
+      <c r="H4" s="211"/>
+      <c r="I4" s="211"/>
+      <c r="J4" s="211"/>
+      <c r="K4" s="211"/>
+      <c r="L4" s="211"/>
+      <c r="M4" s="211"/>
+      <c r="N4" s="211"/>
+      <c r="O4" s="211"/>
+      <c r="P4" s="211"/>
+      <c r="Q4" s="211"/>
+      <c r="R4" s="212"/>
     </row>
     <row r="5" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
@@ -6204,13 +6350,13 @@
       <c r="R5" s="142"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="143" t="s">
+      <c r="A6" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="144">
+      <c r="C6" s="196">
         <v>8</v>
       </c>
       <c r="D6" s="111" t="s">
@@ -6232,9 +6378,9 @@
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="143"/>
-      <c r="B7" s="144"/>
-      <c r="C7" s="144"/>
+      <c r="A7" s="195"/>
+      <c r="B7" s="196"/>
+      <c r="C7" s="196"/>
       <c r="D7" s="112" t="s">
         <v>19</v>
       </c>
@@ -6254,9 +6400,9 @@
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="143"/>
-      <c r="B8" s="144"/>
-      <c r="C8" s="144"/>
+      <c r="A8" s="195"/>
+      <c r="B8" s="196"/>
+      <c r="C8" s="196"/>
       <c r="D8" s="112" t="s">
         <v>21</v>
       </c>
@@ -6276,9 +6422,9 @@
       <c r="R8" s="5"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="143"/>
-      <c r="B9" s="144"/>
-      <c r="C9" s="144"/>
+      <c r="A9" s="195"/>
+      <c r="B9" s="196"/>
+      <c r="C9" s="196"/>
       <c r="D9" s="113" t="s">
         <v>22</v>
       </c>
@@ -6298,13 +6444,13 @@
       <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="161" t="s">
+      <c r="A10" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="162" t="s">
+      <c r="B10" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="162">
+      <c r="C10" s="192">
         <v>8</v>
       </c>
       <c r="D10" s="114" t="s">
@@ -6326,9 +6472,9 @@
       <c r="R10" s="9"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="161"/>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
+      <c r="A11" s="191"/>
+      <c r="B11" s="192"/>
+      <c r="C11" s="192"/>
       <c r="D11" s="115" t="s">
         <v>19</v>
       </c>
@@ -6348,9 +6494,9 @@
       <c r="R11" s="11"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="161"/>
-      <c r="B12" s="162"/>
-      <c r="C12" s="162"/>
+      <c r="A12" s="191"/>
+      <c r="B12" s="192"/>
+      <c r="C12" s="192"/>
       <c r="D12" s="115" t="s">
         <v>21</v>
       </c>
@@ -6370,9 +6516,9 @@
       <c r="R12" s="11"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="161"/>
-      <c r="B13" s="162"/>
-      <c r="C13" s="162"/>
+      <c r="A13" s="191"/>
+      <c r="B13" s="192"/>
+      <c r="C13" s="192"/>
       <c r="D13" s="116" t="s">
         <v>22</v>
       </c>
@@ -6392,13 +6538,13 @@
       <c r="R13" s="13"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="163" t="s">
+      <c r="A14" s="193" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="164">
+      <c r="C14" s="194">
         <v>16</v>
       </c>
       <c r="D14" s="117" t="s">
@@ -6420,9 +6566,9 @@
       <c r="R14" s="15"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="163"/>
-      <c r="B15" s="164"/>
-      <c r="C15" s="164"/>
+      <c r="A15" s="193"/>
+      <c r="B15" s="194"/>
+      <c r="C15" s="194"/>
       <c r="D15" s="118" t="s">
         <v>19</v>
       </c>
@@ -6442,9 +6588,9 @@
       <c r="R15" s="17"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="163"/>
-      <c r="B16" s="164"/>
-      <c r="C16" s="164"/>
+      <c r="A16" s="193"/>
+      <c r="B16" s="194"/>
+      <c r="C16" s="194"/>
       <c r="D16" s="118" t="s">
         <v>21</v>
       </c>
@@ -6464,9 +6610,9 @@
       <c r="R16" s="17"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="163"/>
-      <c r="B17" s="164"/>
-      <c r="C17" s="164"/>
+      <c r="A17" s="193"/>
+      <c r="B17" s="194"/>
+      <c r="C17" s="194"/>
       <c r="D17" s="119" t="s">
         <v>22</v>
       </c>
@@ -6486,13 +6632,13 @@
       <c r="R17" s="19"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="165" t="s">
+      <c r="A18" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="166" t="s">
+      <c r="B18" s="188" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="166">
+      <c r="C18" s="188">
         <v>16</v>
       </c>
       <c r="D18" s="120" t="s">
@@ -6514,9 +6660,9 @@
       <c r="R18" s="21"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="165"/>
-      <c r="B19" s="166"/>
-      <c r="C19" s="166"/>
+      <c r="A19" s="187"/>
+      <c r="B19" s="188"/>
+      <c r="C19" s="188"/>
       <c r="D19" s="121" t="s">
         <v>19</v>
       </c>
@@ -6536,9 +6682,9 @@
       <c r="R19" s="23"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="165"/>
-      <c r="B20" s="166"/>
-      <c r="C20" s="166"/>
+      <c r="A20" s="187"/>
+      <c r="B20" s="188"/>
+      <c r="C20" s="188"/>
       <c r="D20" s="121" t="s">
         <v>21</v>
       </c>
@@ -6558,9 +6704,9 @@
       <c r="R20" s="23"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="165"/>
-      <c r="B21" s="166"/>
-      <c r="C21" s="166"/>
+      <c r="A21" s="187"/>
+      <c r="B21" s="188"/>
+      <c r="C21" s="188"/>
       <c r="D21" s="122" t="s">
         <v>22</v>
       </c>
@@ -6580,13 +6726,13 @@
       <c r="R21" s="25"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="167" t="s">
+      <c r="A22" s="189" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="168" t="s">
+      <c r="B22" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="168">
+      <c r="C22" s="190">
         <v>32</v>
       </c>
       <c r="D22" s="123" t="s">
@@ -6608,9 +6754,9 @@
       <c r="R22" s="27"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="167"/>
-      <c r="B23" s="168"/>
-      <c r="C23" s="168"/>
+      <c r="A23" s="189"/>
+      <c r="B23" s="190"/>
+      <c r="C23" s="190"/>
       <c r="D23" s="124" t="s">
         <v>19</v>
       </c>
@@ -6630,9 +6776,9 @@
       <c r="R23" s="29"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="167"/>
-      <c r="B24" s="168"/>
-      <c r="C24" s="168"/>
+      <c r="A24" s="189"/>
+      <c r="B24" s="190"/>
+      <c r="C24" s="190"/>
       <c r="D24" s="124" t="s">
         <v>21</v>
       </c>
@@ -6652,9 +6798,9 @@
       <c r="R24" s="29"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="167"/>
-      <c r="B25" s="168"/>
-      <c r="C25" s="168"/>
+      <c r="A25" s="189"/>
+      <c r="B25" s="190"/>
+      <c r="C25" s="190"/>
       <c r="D25" s="125" t="s">
         <v>22</v>
       </c>
@@ -6674,13 +6820,13 @@
       <c r="R25" s="31"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="169" t="s">
+      <c r="A26" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="170" t="s">
+      <c r="B26" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="170">
+      <c r="C26" s="184">
         <v>32</v>
       </c>
       <c r="D26" s="126" t="s">
@@ -6702,9 +6848,9 @@
       <c r="R26" s="33"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="169"/>
-      <c r="B27" s="170"/>
-      <c r="C27" s="170"/>
+      <c r="A27" s="183"/>
+      <c r="B27" s="184"/>
+      <c r="C27" s="184"/>
       <c r="D27" s="127" t="s">
         <v>19</v>
       </c>
@@ -6724,9 +6870,9 @@
       <c r="R27" s="35"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="169"/>
-      <c r="B28" s="170"/>
-      <c r="C28" s="170"/>
+      <c r="A28" s="183"/>
+      <c r="B28" s="184"/>
+      <c r="C28" s="184"/>
       <c r="D28" s="127" t="s">
         <v>21</v>
       </c>
@@ -6746,9 +6892,9 @@
       <c r="R28" s="35"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="169"/>
-      <c r="B29" s="170"/>
-      <c r="C29" s="170"/>
+      <c r="A29" s="183"/>
+      <c r="B29" s="184"/>
+      <c r="C29" s="184"/>
       <c r="D29" s="128" t="s">
         <v>22</v>
       </c>
@@ -6768,13 +6914,13 @@
       <c r="R29" s="37"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="171" t="s">
+      <c r="A30" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="172" t="s">
+      <c r="B30" s="186" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="172">
+      <c r="C30" s="186">
         <v>32</v>
       </c>
       <c r="D30" s="129" t="s">
@@ -6796,9 +6942,9 @@
       <c r="R30" s="39"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="171"/>
-      <c r="B31" s="172"/>
-      <c r="C31" s="172"/>
+      <c r="A31" s="185"/>
+      <c r="B31" s="186"/>
+      <c r="C31" s="186"/>
       <c r="D31" s="130" t="s">
         <v>19</v>
       </c>
@@ -6818,9 +6964,9 @@
       <c r="R31" s="41"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="171"/>
-      <c r="B32" s="172"/>
-      <c r="C32" s="172"/>
+      <c r="A32" s="185"/>
+      <c r="B32" s="186"/>
+      <c r="C32" s="186"/>
       <c r="D32" s="130" t="s">
         <v>21</v>
       </c>
@@ -6840,9 +6986,9 @@
       <c r="R32" s="41"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="171"/>
-      <c r="B33" s="172"/>
-      <c r="C33" s="172"/>
+      <c r="A33" s="185"/>
+      <c r="B33" s="186"/>
+      <c r="C33" s="186"/>
       <c r="D33" s="131" t="s">
         <v>22</v>
       </c>
@@ -6862,13 +7008,13 @@
       <c r="R33" s="55"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="173" t="s">
+      <c r="A34" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="174" t="s">
+      <c r="B34" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="175" t="s">
+      <c r="C34" s="179" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="132" t="s">
@@ -6890,9 +7036,9 @@
       <c r="R34" s="43"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="173"/>
-      <c r="B35" s="174"/>
-      <c r="C35" s="175"/>
+      <c r="A35" s="177"/>
+      <c r="B35" s="178"/>
+      <c r="C35" s="179"/>
       <c r="D35" s="133" t="s">
         <v>19</v>
       </c>
@@ -6912,9 +7058,9 @@
       <c r="R35" s="45"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="173"/>
-      <c r="B36" s="174"/>
-      <c r="C36" s="175"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="178"/>
+      <c r="C36" s="179"/>
       <c r="D36" s="133" t="s">
         <v>21</v>
       </c>
@@ -6934,9 +7080,9 @@
       <c r="R36" s="45"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="173"/>
-      <c r="B37" s="174"/>
-      <c r="C37" s="174"/>
+      <c r="A37" s="177"/>
+      <c r="B37" s="178"/>
+      <c r="C37" s="178"/>
       <c r="D37" s="134" t="s">
         <v>22</v>
       </c>
@@ -6956,13 +7102,13 @@
       <c r="R37" s="57"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="176" t="s">
+      <c r="A38" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="177" t="s">
+      <c r="B38" s="181" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="178" t="s">
+      <c r="C38" s="182" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="135" t="s">
@@ -6984,9 +7130,9 @@
       <c r="R38" s="47"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="176"/>
-      <c r="B39" s="177"/>
-      <c r="C39" s="178"/>
+      <c r="A39" s="180"/>
+      <c r="B39" s="181"/>
+      <c r="C39" s="182"/>
       <c r="D39" s="136" t="s">
         <v>19</v>
       </c>
@@ -7006,9 +7152,9 @@
       <c r="R39" s="49"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="176"/>
-      <c r="B40" s="177"/>
-      <c r="C40" s="178"/>
+      <c r="A40" s="180"/>
+      <c r="B40" s="181"/>
+      <c r="C40" s="182"/>
       <c r="D40" s="136" t="s">
         <v>21</v>
       </c>
@@ -7028,9 +7174,9 @@
       <c r="R40" s="49"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="176"/>
-      <c r="B41" s="177"/>
-      <c r="C41" s="177"/>
+      <c r="A41" s="180"/>
+      <c r="B41" s="181"/>
+      <c r="C41" s="181"/>
       <c r="D41" s="137" t="s">
         <v>22</v>
       </c>
@@ -7050,13 +7196,13 @@
       <c r="R41" s="59"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="179" t="s">
+      <c r="A42" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="181" t="s">
+      <c r="B42" s="170" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="182" t="s">
+      <c r="C42" s="171" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="138" t="s">
@@ -7078,9 +7224,9 @@
       <c r="R42" s="51"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="179"/>
-      <c r="B43" s="181"/>
-      <c r="C43" s="182"/>
+      <c r="A43" s="168"/>
+      <c r="B43" s="170"/>
+      <c r="C43" s="171"/>
       <c r="D43" s="139" t="s">
         <v>19</v>
       </c>
@@ -7100,9 +7246,9 @@
       <c r="R43" s="53"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="179"/>
-      <c r="B44" s="181"/>
-      <c r="C44" s="182"/>
+      <c r="A44" s="168"/>
+      <c r="B44" s="170"/>
+      <c r="C44" s="171"/>
       <c r="D44" s="139" t="s">
         <v>21</v>
       </c>
@@ -7122,9 +7268,9 @@
       <c r="R44" s="53"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="180"/>
-      <c r="B45" s="181"/>
-      <c r="C45" s="181"/>
+      <c r="A45" s="169"/>
+      <c r="B45" s="170"/>
+      <c r="C45" s="170"/>
       <c r="D45" s="139" t="s">
         <v>22</v>
       </c>
@@ -7144,56 +7290,56 @@
       <c r="R45" s="53"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="183" t="s">
+      <c r="A46" s="172" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="184"/>
-      <c r="C46" s="184"/>
-      <c r="D46" s="185"/>
-      <c r="E46" s="186"/>
-      <c r="F46" s="188"/>
-      <c r="G46" s="188"/>
-      <c r="H46" s="188"/>
-      <c r="I46" s="192" t="s">
+      <c r="B46" s="173"/>
+      <c r="C46" s="173"/>
+      <c r="D46" s="174"/>
+      <c r="E46" s="175"/>
+      <c r="F46" s="147"/>
+      <c r="G46" s="147"/>
+      <c r="H46" s="147"/>
+      <c r="I46" s="166" t="s">
         <v>1</v>
       </c>
-      <c r="J46" s="188"/>
-      <c r="K46" s="188"/>
-      <c r="L46" s="188"/>
-      <c r="M46" s="188"/>
-      <c r="N46" s="188"/>
-      <c r="O46" s="188"/>
-      <c r="P46" s="188"/>
-      <c r="Q46" s="188"/>
-      <c r="R46" s="190"/>
+      <c r="J46" s="147"/>
+      <c r="K46" s="147"/>
+      <c r="L46" s="147"/>
+      <c r="M46" s="147"/>
+      <c r="N46" s="147"/>
+      <c r="O46" s="147"/>
+      <c r="P46" s="147"/>
+      <c r="Q46" s="147"/>
+      <c r="R46" s="164"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="183"/>
-      <c r="B47" s="184"/>
-      <c r="C47" s="184"/>
-      <c r="D47" s="185"/>
-      <c r="E47" s="187"/>
-      <c r="F47" s="189"/>
-      <c r="G47" s="189"/>
-      <c r="H47" s="189"/>
-      <c r="I47" s="193"/>
-      <c r="J47" s="189"/>
-      <c r="K47" s="189"/>
-      <c r="L47" s="189"/>
-      <c r="M47" s="189"/>
-      <c r="N47" s="189"/>
-      <c r="O47" s="189"/>
-      <c r="P47" s="189"/>
-      <c r="Q47" s="189"/>
-      <c r="R47" s="191"/>
+      <c r="A47" s="172"/>
+      <c r="B47" s="173"/>
+      <c r="C47" s="173"/>
+      <c r="D47" s="174"/>
+      <c r="E47" s="176"/>
+      <c r="F47" s="148"/>
+      <c r="G47" s="148"/>
+      <c r="H47" s="148"/>
+      <c r="I47" s="167"/>
+      <c r="J47" s="148"/>
+      <c r="K47" s="148"/>
+      <c r="L47" s="148"/>
+      <c r="M47" s="148"/>
+      <c r="N47" s="148"/>
+      <c r="O47" s="148"/>
+      <c r="P47" s="148"/>
+      <c r="Q47" s="148"/>
+      <c r="R47" s="165"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="197" t="s">
+      <c r="A48" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="198"/>
-      <c r="C48" s="198"/>
-      <c r="D48" s="199"/>
+      <c r="B48" s="150"/>
+      <c r="C48" s="150"/>
+      <c r="D48" s="151"/>
       <c r="E48" s="104"/>
       <c r="F48" s="65"/>
       <c r="G48" s="65"/>
@@ -7210,12 +7356,12 @@
       <c r="R48" s="66"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="200" t="s">
+      <c r="A49" s="152" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="201"/>
-      <c r="C49" s="201"/>
-      <c r="D49" s="202"/>
+      <c r="B49" s="153"/>
+      <c r="C49" s="153"/>
+      <c r="D49" s="154"/>
       <c r="E49" s="105"/>
       <c r="F49" s="63"/>
       <c r="G49" s="63"/>
@@ -7232,12 +7378,12 @@
       <c r="R49" s="64"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="203" t="s">
+      <c r="A50" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="204"/>
-      <c r="C50" s="204"/>
-      <c r="D50" s="205"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="156"/>
+      <c r="D50" s="157"/>
       <c r="E50" s="106"/>
       <c r="F50" s="67"/>
       <c r="G50" s="67"/>
@@ -7254,12 +7400,12 @@
       <c r="R50" s="68"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="206" t="s">
+      <c r="A51" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="207"/>
-      <c r="C51" s="207"/>
-      <c r="D51" s="208"/>
+      <c r="B51" s="159"/>
+      <c r="C51" s="159"/>
+      <c r="D51" s="160"/>
       <c r="E51" s="107"/>
       <c r="F51" s="69"/>
       <c r="G51" s="69"/>
@@ -7276,12 +7422,12 @@
       <c r="R51" s="70"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="209" t="s">
+      <c r="A52" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="210"/>
-      <c r="C52" s="210"/>
-      <c r="D52" s="211"/>
+      <c r="B52" s="162"/>
+      <c r="C52" s="162"/>
+      <c r="D52" s="163"/>
       <c r="E52" s="108"/>
       <c r="F52" s="71"/>
       <c r="G52" s="71"/>
@@ -7298,12 +7444,12 @@
       <c r="R52" s="72"/>
     </row>
     <row r="53" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="194" t="s">
+      <c r="A53" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="195"/>
-      <c r="C53" s="195"/>
-      <c r="D53" s="196"/>
+      <c r="B53" s="145"/>
+      <c r="C53" s="145"/>
+      <c r="D53" s="146"/>
       <c r="E53" s="109"/>
       <c r="F53" s="73"/>
       <c r="G53" s="73"/>
@@ -7322,11 +7468,41 @@
     <row r="54" spans="1:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="N46:N47"/>
-    <mergeCell ref="O46:O47"/>
-    <mergeCell ref="P46:P47"/>
-    <mergeCell ref="Q46:Q47"/>
-    <mergeCell ref="R46:R47"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="E2:R3"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="A46:D47"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
     <mergeCell ref="A2:D4"/>
     <mergeCell ref="E4:R4"/>
     <mergeCell ref="A1:I1"/>
@@ -7343,41 +7519,11 @@
     <mergeCell ref="B42:B45"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="E2:R3"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="A46:D47"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="N46:N47"/>
+    <mergeCell ref="O46:O47"/>
+    <mergeCell ref="P46:P47"/>
+    <mergeCell ref="Q46:Q47"/>
+    <mergeCell ref="R46:R47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>